<commit_message>
method call and class member access
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="pc-basics" sheetId="1" r:id="rId1"/>
@@ -14,34 +14,35 @@
     <sheet name="methods" sheetId="5" r:id="rId5"/>
     <sheet name="tech-terms" sheetId="6" r:id="rId6"/>
     <sheet name="references-latest" sheetId="28" r:id="rId7"/>
-    <sheet name="method-calls" sheetId="7" r:id="rId8"/>
-    <sheet name="variable-scope" sheetId="8" r:id="rId9"/>
-    <sheet name="references" sheetId="9" r:id="rId10"/>
-    <sheet name="pass-by-value" sheetId="10" r:id="rId11"/>
-    <sheet name="operator" sheetId="11" r:id="rId12"/>
-    <sheet name="control-flow" sheetId="12" r:id="rId13"/>
-    <sheet name="constructor" sheetId="13" r:id="rId14"/>
-    <sheet name="in-heritance" sheetId="14" r:id="rId15"/>
-    <sheet name="practice" sheetId="15" r:id="rId16"/>
-    <sheet name="interface-abstract" sheetId="16" r:id="rId17"/>
-    <sheet name="inheritance-access-priv-dto" sheetId="17" r:id="rId18"/>
-    <sheet name="poly-final" sheetId="18" r:id="rId19"/>
-    <sheet name="static" sheetId="19" r:id="rId20"/>
-    <sheet name="array" sheetId="20" r:id="rId21"/>
-    <sheet name="String" sheetId="21" r:id="rId22"/>
-    <sheet name="exception_handling" sheetId="22" r:id="rId23"/>
-    <sheet name="threads" sheetId="23" r:id="rId24"/>
-    <sheet name="collection" sheetId="24" r:id="rId25"/>
-    <sheet name="collection2" sheetId="25" r:id="rId26"/>
-    <sheet name="col-unique" sheetId="26" r:id="rId27"/>
-    <sheet name="file" sheetId="27" r:id="rId28"/>
+    <sheet name="program-communication" sheetId="29" r:id="rId8"/>
+    <sheet name="method-calls" sheetId="7" r:id="rId9"/>
+    <sheet name="variable-scope" sheetId="8" r:id="rId10"/>
+    <sheet name="references" sheetId="9" r:id="rId11"/>
+    <sheet name="pass-by-value" sheetId="10" r:id="rId12"/>
+    <sheet name="operator" sheetId="11" r:id="rId13"/>
+    <sheet name="control-flow" sheetId="12" r:id="rId14"/>
+    <sheet name="constructor" sheetId="13" r:id="rId15"/>
+    <sheet name="in-heritance" sheetId="14" r:id="rId16"/>
+    <sheet name="practice" sheetId="15" r:id="rId17"/>
+    <sheet name="interface-abstract" sheetId="16" r:id="rId18"/>
+    <sheet name="inheritance-access-priv-dto" sheetId="17" r:id="rId19"/>
+    <sheet name="poly-final" sheetId="18" r:id="rId20"/>
+    <sheet name="static" sheetId="19" r:id="rId21"/>
+    <sheet name="array" sheetId="20" r:id="rId22"/>
+    <sheet name="String" sheetId="21" r:id="rId23"/>
+    <sheet name="exception_handling" sheetId="22" r:id="rId24"/>
+    <sheet name="threads" sheetId="23" r:id="rId25"/>
+    <sheet name="collection" sheetId="24" r:id="rId26"/>
+    <sheet name="collection2" sheetId="25" r:id="rId27"/>
+    <sheet name="col-unique" sheetId="26" r:id="rId28"/>
+    <sheet name="file" sheetId="27" r:id="rId29"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6159" uniqueCount="3250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6205" uniqueCount="3276">
   <si>
     <t>USER</t>
   </si>
@@ -10056,6 +10057,85 @@
   </si>
   <si>
     <t>META</t>
+  </si>
+  <si>
+    <t>applyLoan()</t>
+  </si>
+  <si>
+    <t>LoanOfficer</t>
+  </si>
+  <si>
+    <t>loanOfficer</t>
+  </si>
+  <si>
+    <t>BankManager</t>
+  </si>
+  <si>
+    <t>branchManager</t>
+  </si>
+  <si>
+    <t>creditScore</t>
+  </si>
+  <si>
+    <t>if(credit score is greater than 700</t>
+  </si>
+  <si>
+    <t>verifyLoan(  credit score)</t>
+  </si>
+  <si>
+    <t>processLoan(salary , creditscore, loan, years)</t>
+  </si>
+  <si>
+    <t>check with Bank manager</t>
+  </si>
+  <si>
+    <t>processLoan(salary,creditscore
+, 100000,30)</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>if(salary is greater than salaryMinimum)</t>
+  </si>
+  <si>
+    <t>loanSalaryMin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessing information (variables) and actions (methods ):  </t>
+  </si>
+  <si>
+    <t>within same class : direct access</t>
+  </si>
+  <si>
+    <t>outside class : create reference to the other program</t>
+  </si>
+  <si>
+    <t>Communication between 2 programs</t>
+  </si>
+  <si>
+    <t>1) create reference to other program</t>
+  </si>
+  <si>
+    <t>2) call methods of the other program</t>
+  </si>
+  <si>
+    <t>MODULAR</t>
+  </si>
+  <si>
+    <t>Reference : LoanOfficer lo=new LoanOfficer();</t>
+  </si>
+  <si>
+    <t>lo = reference variable</t>
+  </si>
+  <si>
+    <t>using reference variableand dot operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> u can access variable and methods from LoanOfficer program</t>
   </si>
 </sst>
 </file>
@@ -10661,7 +10741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="348">
+  <cellXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -11344,6 +11424,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11352,12 +11450,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11372,18 +11464,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13092,6 +13200,439 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D3:H121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="4:6">
+      <c r="D3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6">
+      <c r="D4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6">
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6">
+      <c r="E7" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6">
+      <c r="E8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="E10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6">
+      <c r="F11" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6">
+      <c r="E12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6">
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6">
+      <c r="D14" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6">
+      <c r="D15" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5">
+      <c r="E21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5">
+      <c r="E22" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5">
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5">
+      <c r="D25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5">
+      <c r="D27" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5">
+      <c r="E28" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5">
+      <c r="E29" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5">
+      <c r="E31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5">
+      <c r="D32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5">
+      <c r="D35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5">
+      <c r="D36" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5">
+      <c r="D37" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5">
+      <c r="D38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5">
+      <c r="D39" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5">
+      <c r="E40" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5">
+      <c r="D41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5">
+      <c r="D42" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5">
+      <c r="D43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5">
+      <c r="D44" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5">
+      <c r="D45" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5">
+      <c r="E46" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5">
+      <c r="D47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5">
+      <c r="D48" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8">
+      <c r="D51" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8">
+      <c r="E52" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8">
+      <c r="F53" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="54" spans="4:8">
+      <c r="G54" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="56" spans="4:8">
+      <c r="G56" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="57" spans="4:8">
+      <c r="G57" t="s">
+        <v>371</v>
+      </c>
+      <c r="H57" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="58" spans="4:8">
+      <c r="G58" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="60" spans="4:8">
+      <c r="G60" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="62" spans="4:8">
+      <c r="G62" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="63" spans="4:8">
+      <c r="F63" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="4:8">
+      <c r="E64" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="4:7">
+      <c r="D66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="4:7">
+      <c r="D68" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="69" spans="4:7">
+      <c r="D69" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="70" spans="4:7">
+      <c r="D70" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="75" spans="4:7">
+      <c r="D75" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="76" spans="4:7">
+      <c r="E76" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="77" spans="4:7">
+      <c r="E77" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="78" spans="4:7">
+      <c r="F78" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="79" spans="4:7">
+      <c r="G79" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="80" spans="4:7">
+      <c r="F80" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="4:5">
+      <c r="E81" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="4:5">
+      <c r="D82" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="4:5">
+      <c r="D83" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="88" spans="4:5">
+      <c r="D88" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="91" spans="4:5">
+      <c r="D91" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="92" spans="4:5">
+      <c r="D92" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="93" spans="4:5">
+      <c r="D93" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="96" spans="4:5">
+      <c r="D96" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="101" spans="4:5">
+      <c r="D101" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5">
+      <c r="E102" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5">
+      <c r="D103" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="104" spans="4:5">
+      <c r="E104" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="105" spans="4:5">
+      <c r="D105" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="106" spans="4:5">
+      <c r="E106" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="107" spans="4:5">
+      <c r="E107" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="108" spans="4:5">
+      <c r="E108" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="111" spans="4:5">
+      <c r="E111" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="112" spans="4:5">
+      <c r="D112" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6">
+      <c r="E113" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6">
+      <c r="E114" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="115" spans="4:6">
+      <c r="F115" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="116" spans="4:6">
+      <c r="F116" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="117" spans="4:6">
+      <c r="F117" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="119" spans="4:6">
+      <c r="F119" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="120" spans="4:6">
+      <c r="E120" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="121" spans="4:6">
+      <c r="D121" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:T200"/>
   <sheetViews>
     <sheetView topLeftCell="A178" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -15634,7 +16175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P157"/>
   <sheetViews>
@@ -17672,7 +18213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:C67"/>
   <sheetViews>
@@ -17935,7 +18476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O187"/>
   <sheetViews>
@@ -19270,7 +19811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P229"/>
   <sheetViews>
@@ -20833,7 +21374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:V272"/>
   <sheetViews>
@@ -22469,7 +23010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E3:E15"/>
   <sheetViews>
@@ -22539,7 +23080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N91"/>
   <sheetViews>
@@ -22986,7 +23527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C105"/>
   <sheetViews>
@@ -23464,321 +24005,6 @@
     <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>943</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G93"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G94"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="C16" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="B17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="B18" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="B19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="B24" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="B25" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="B28" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="B29" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="B33" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="B34" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="B40" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="B42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="B45" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="B47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="B61" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="B69" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="C70" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="B71" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="G91" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="B93" t="s">
-        <v>992</v>
       </c>
     </row>
   </sheetData>
@@ -25156,6 +25382,321 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G93"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G94"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="B33" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="B34" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="B40" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="B42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="B45" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="B61" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="C70" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="B71" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="G91" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="B93" t="s">
+        <v>992</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R293"/>
   <sheetViews>
@@ -25226,7 +25767,7 @@
       </c>
       <c r="L3" s="47"/>
       <c r="M3" s="48"/>
-      <c r="N3" s="336" t="s">
+      <c r="N3" s="342" t="s">
         <v>2980</v>
       </c>
       <c r="O3" s="51"/>
@@ -25255,7 +25796,7 @@
       <c r="K4" s="51"/>
       <c r="L4" s="50"/>
       <c r="M4" s="51"/>
-      <c r="N4" s="337"/>
+      <c r="N4" s="335"/>
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
       <c r="Q4" s="52"/>
@@ -25281,7 +25822,7 @@
       <c r="M5" s="51" t="s">
         <v>559</v>
       </c>
-      <c r="N5" s="337"/>
+      <c r="N5" s="335"/>
       <c r="O5" s="51"/>
       <c r="P5" s="51"/>
       <c r="Q5" s="52"/>
@@ -25303,7 +25844,7 @@
       <c r="M6" s="54">
         <v>12345</v>
       </c>
-      <c r="N6" s="337"/>
+      <c r="N6" s="335"/>
       <c r="O6" s="51"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="52"/>
@@ -25321,7 +25862,7 @@
       <c r="K7" s="51"/>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
-      <c r="N7" s="337"/>
+      <c r="N7" s="335"/>
       <c r="O7" s="51"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="52"/>
@@ -25341,7 +25882,7 @@
       </c>
       <c r="L8" s="47"/>
       <c r="M8" s="48"/>
-      <c r="N8" s="337"/>
+      <c r="N8" s="335"/>
       <c r="O8" s="51"/>
       <c r="P8" s="51"/>
       <c r="Q8" s="52"/>
@@ -25359,7 +25900,7 @@
       <c r="K9" s="51"/>
       <c r="L9" s="50"/>
       <c r="M9" s="51"/>
-      <c r="N9" s="337"/>
+      <c r="N9" s="335"/>
       <c r="O9" s="51"/>
       <c r="P9" s="51"/>
       <c r="Q9" s="52"/>
@@ -25376,7 +25917,7 @@
       <c r="M10" s="51" t="s">
         <v>524</v>
       </c>
-      <c r="N10" s="337"/>
+      <c r="N10" s="335"/>
       <c r="O10" s="51"/>
       <c r="P10" s="51"/>
       <c r="Q10" s="52"/>
@@ -25396,7 +25937,7 @@
       <c r="M11" s="54">
         <v>12346</v>
       </c>
-      <c r="N11" s="338"/>
+      <c r="N11" s="336"/>
       <c r="O11" s="51"/>
       <c r="P11" s="51"/>
       <c r="Q11" s="52"/>
@@ -28719,7 +29260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P284"/>
   <sheetViews>
@@ -31731,7 +32272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O366"/>
   <sheetViews>
@@ -35362,7 +35903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W353"/>
   <sheetViews>
@@ -37577,7 +38118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:P245"/>
   <sheetViews>
@@ -37726,24 +38267,24 @@
     <row r="17" spans="1:14" s="108" customFormat="1"/>
     <row r="22" spans="1:14" ht="15.75" thickBot="1">
       <c r="A22" s="106"/>
-      <c r="B22" s="339" t="s">
+      <c r="B22" s="343" t="s">
         <v>1251</v>
       </c>
-      <c r="C22" s="339"/>
+      <c r="C22" s="343"/>
       <c r="D22" s="106"/>
       <c r="E22" s="106"/>
-      <c r="F22" s="339" t="s">
+      <c r="F22" s="343" t="s">
         <v>1355</v>
       </c>
-      <c r="G22" s="339"/>
-      <c r="H22" s="339"/>
+      <c r="G22" s="343"/>
+      <c r="H22" s="343"/>
       <c r="I22" s="106"/>
       <c r="J22" s="106"/>
-      <c r="K22" s="339" t="s">
+      <c r="K22" s="343" t="s">
         <v>1253</v>
       </c>
-      <c r="L22" s="339"/>
-      <c r="M22" s="339"/>
+      <c r="L22" s="343"/>
+      <c r="M22" s="343"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14">
@@ -40127,7 +40668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF304"/>
   <sheetViews>
@@ -40301,35 +40842,35 @@
       </c>
     </row>
     <row r="8" spans="1:31">
-      <c r="B8" s="341" t="s">
+      <c r="B8" s="345" t="s">
         <v>3070</v>
       </c>
-      <c r="C8" s="341"/>
-      <c r="F8" s="341" t="s">
+      <c r="C8" s="345"/>
+      <c r="F8" s="345" t="s">
         <v>3071</v>
       </c>
-      <c r="G8" s="341"/>
-      <c r="I8" s="341" t="s">
+      <c r="G8" s="345"/>
+      <c r="I8" s="345" t="s">
         <v>3071</v>
       </c>
-      <c r="J8" s="341"/>
+      <c r="J8" s="345"/>
       <c r="M8" s="249" t="s">
         <v>3128</v>
       </c>
     </row>
     <row r="9" spans="1:31">
-      <c r="F9" s="341" t="s">
+      <c r="F9" s="345" t="s">
         <v>3072</v>
       </c>
-      <c r="G9" s="341"/>
-      <c r="I9" s="341" t="s">
+      <c r="G9" s="345"/>
+      <c r="I9" s="345" t="s">
         <v>3073</v>
       </c>
-      <c r="J9" s="341"/>
-      <c r="M9" s="342" t="s">
+      <c r="J9" s="345"/>
+      <c r="M9" s="346" t="s">
         <v>3071</v>
       </c>
-      <c r="N9" s="342"/>
+      <c r="N9" s="346"/>
     </row>
     <row r="10" spans="1:31">
       <c r="M10" s="314" t="s">
@@ -40338,19 +40879,19 @@
       <c r="N10" s="314"/>
     </row>
     <row r="11" spans="1:31">
-      <c r="E11" s="340" t="s">
+      <c r="E11" s="344" t="s">
         <v>3075</v>
       </c>
-      <c r="F11" s="340"/>
-      <c r="G11" s="340"/>
-      <c r="H11" s="340"/>
-      <c r="I11" s="340"/>
-      <c r="J11" s="340"/>
-      <c r="K11" s="340"/>
-      <c r="L11" s="340"/>
-      <c r="M11" s="340"/>
-      <c r="N11" s="340"/>
-      <c r="O11" s="340"/>
+      <c r="F11" s="344"/>
+      <c r="G11" s="344"/>
+      <c r="H11" s="344"/>
+      <c r="I11" s="344"/>
+      <c r="J11" s="344"/>
+      <c r="K11" s="344"/>
+      <c r="L11" s="344"/>
+      <c r="M11" s="344"/>
+      <c r="N11" s="344"/>
+      <c r="O11" s="344"/>
     </row>
     <row r="12" spans="1:31">
       <c r="A12" t="s">
@@ -43650,7 +44191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:U125"/>
   <sheetViews>
@@ -43973,7 +44514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S54"/>
   <sheetViews>
@@ -44110,11 +44651,11 @@
       <c r="L6" s="43" t="s">
         <v>1527</v>
       </c>
-      <c r="M6" s="343" t="s">
+      <c r="M6" s="347" t="s">
         <v>1528</v>
       </c>
-      <c r="N6" s="343"/>
-      <c r="O6" s="343"/>
+      <c r="N6" s="347"/>
+      <c r="O6" s="347"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
@@ -44522,7 +45063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:L85"/>
   <sheetViews>
@@ -44880,8 +45421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D130" sqref="D130"/>
+    <sheetView topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="J121" sqref="J121:J135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -45641,10 +46182,10 @@
       </c>
       <c r="G121" s="30"/>
       <c r="H121" s="31"/>
-      <c r="I121" s="344" t="s">
+      <c r="I121" s="334" t="s">
         <v>3245</v>
       </c>
-      <c r="J121" s="344" t="s">
+      <c r="J121" s="334" t="s">
         <v>3249</v>
       </c>
       <c r="K121" s="27"/>
@@ -45660,8 +46201,8 @@
       <c r="H122" s="27" t="s">
         <v>559</v>
       </c>
-      <c r="I122" s="337"/>
-      <c r="J122" s="337"/>
+      <c r="I122" s="335"/>
+      <c r="J122" s="335"/>
       <c r="K122" s="27"/>
       <c r="L122" s="27"/>
       <c r="M122" s="34"/>
@@ -45675,8 +46216,8 @@
       <c r="H123" s="27">
         <v>19</v>
       </c>
-      <c r="I123" s="337"/>
-      <c r="J123" s="337"/>
+      <c r="I123" s="335"/>
+      <c r="J123" s="335"/>
       <c r="K123" s="27"/>
       <c r="L123" s="27"/>
       <c r="M123" s="34"/>
@@ -45690,8 +46231,8 @@
       <c r="H124" s="36" t="s">
         <v>2160</v>
       </c>
-      <c r="I124" s="337"/>
-      <c r="J124" s="337"/>
+      <c r="I124" s="335"/>
+      <c r="J124" s="335"/>
       <c r="K124" s="27"/>
       <c r="L124" s="27"/>
       <c r="M124" s="34"/>
@@ -45701,8 +46242,8 @@
       <c r="F125" s="27"/>
       <c r="G125" s="27"/>
       <c r="H125" s="27"/>
-      <c r="I125" s="337"/>
-      <c r="J125" s="337"/>
+      <c r="I125" s="335"/>
+      <c r="J125" s="335"/>
       <c r="K125" s="27"/>
       <c r="L125" s="27"/>
       <c r="M125" s="34"/>
@@ -45715,8 +46256,8 @@
       <c r="F126" s="27"/>
       <c r="G126" s="27"/>
       <c r="H126" s="27"/>
-      <c r="I126" s="337"/>
-      <c r="J126" s="337"/>
+      <c r="I126" s="335"/>
+      <c r="J126" s="335"/>
       <c r="K126" s="27"/>
       <c r="L126" s="27"/>
       <c r="M126" s="34"/>
@@ -45728,8 +46269,8 @@
       </c>
       <c r="G127" s="30"/>
       <c r="H127" s="31"/>
-      <c r="I127" s="337"/>
-      <c r="J127" s="337"/>
+      <c r="I127" s="335"/>
+      <c r="J127" s="335"/>
       <c r="K127" s="27"/>
       <c r="L127" s="27"/>
       <c r="M127" s="34"/>
@@ -45743,8 +46284,8 @@
       <c r="H128" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="I128" s="337"/>
-      <c r="J128" s="337"/>
+      <c r="I128" s="335"/>
+      <c r="J128" s="335"/>
       <c r="K128" s="27"/>
       <c r="L128" s="27"/>
       <c r="M128" s="34"/>
@@ -45758,8 +46299,8 @@
       <c r="H129" s="27">
         <v>20</v>
       </c>
-      <c r="I129" s="337"/>
-      <c r="J129" s="337"/>
+      <c r="I129" s="335"/>
+      <c r="J129" s="335"/>
       <c r="K129" s="27"/>
       <c r="L129" s="27"/>
       <c r="M129" s="34"/>
@@ -45773,8 +46314,8 @@
       <c r="H130" s="36" t="s">
         <v>3241</v>
       </c>
-      <c r="I130" s="337"/>
-      <c r="J130" s="337"/>
+      <c r="I130" s="335"/>
+      <c r="J130" s="335"/>
       <c r="K130" s="27"/>
       <c r="L130" s="27"/>
       <c r="M130" s="34"/>
@@ -45784,8 +46325,8 @@
       <c r="F131" s="27"/>
       <c r="G131" s="27"/>
       <c r="H131" s="27"/>
-      <c r="I131" s="337"/>
-      <c r="J131" s="337"/>
+      <c r="I131" s="335"/>
+      <c r="J131" s="335"/>
       <c r="K131" s="27"/>
       <c r="L131" s="27"/>
       <c r="M131" s="34"/>
@@ -45797,8 +46338,8 @@
       </c>
       <c r="G132" s="30"/>
       <c r="H132" s="31"/>
-      <c r="I132" s="337"/>
-      <c r="J132" s="337"/>
+      <c r="I132" s="335"/>
+      <c r="J132" s="335"/>
       <c r="K132" s="27"/>
       <c r="L132" s="27"/>
       <c r="M132" s="34"/>
@@ -45812,8 +46353,8 @@
       <c r="H133" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="I133" s="337"/>
-      <c r="J133" s="337"/>
+      <c r="I133" s="335"/>
+      <c r="J133" s="335"/>
       <c r="K133" s="27"/>
       <c r="L133" s="27"/>
       <c r="M133" s="34"/>
@@ -45827,8 +46368,8 @@
       <c r="H134" s="27">
         <v>18</v>
       </c>
-      <c r="I134" s="337"/>
-      <c r="J134" s="337"/>
+      <c r="I134" s="335"/>
+      <c r="J134" s="335"/>
       <c r="K134" s="27"/>
       <c r="L134" s="27"/>
       <c r="M134" s="34"/>
@@ -45842,8 +46383,8 @@
       <c r="H135" s="36" t="s">
         <v>3242</v>
       </c>
-      <c r="I135" s="338"/>
-      <c r="J135" s="338"/>
+      <c r="I135" s="336"/>
+      <c r="J135" s="336"/>
       <c r="K135" s="27"/>
       <c r="L135" s="27"/>
       <c r="M135" s="34"/>
@@ -45923,8 +46464,8 @@
       <c r="H147" s="31" t="s">
         <v>3248</v>
       </c>
-      <c r="I147" s="345"/>
-      <c r="J147" s="345"/>
+      <c r="I147" s="337"/>
+      <c r="J147" s="337"/>
       <c r="K147" s="27"/>
       <c r="L147" s="27"/>
       <c r="M147" s="34"/>
@@ -45938,8 +46479,8 @@
       <c r="H148" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="I148" s="346"/>
-      <c r="J148" s="346"/>
+      <c r="I148" s="338"/>
+      <c r="J148" s="338"/>
       <c r="K148" s="27"/>
       <c r="L148" s="27"/>
       <c r="M148" s="34"/>
@@ -45953,8 +46494,8 @@
       <c r="H149" s="27">
         <v>19</v>
       </c>
-      <c r="I149" s="346"/>
-      <c r="J149" s="346"/>
+      <c r="I149" s="338"/>
+      <c r="J149" s="338"/>
       <c r="K149" s="27"/>
       <c r="L149" s="27"/>
       <c r="M149" s="34"/>
@@ -45968,8 +46509,8 @@
       <c r="H150" s="36" t="s">
         <v>2160</v>
       </c>
-      <c r="I150" s="346"/>
-      <c r="J150" s="346"/>
+      <c r="I150" s="338"/>
+      <c r="J150" s="338"/>
       <c r="K150" s="27"/>
       <c r="L150" s="27"/>
       <c r="M150" s="34"/>
@@ -45979,8 +46520,8 @@
       <c r="F151" s="27"/>
       <c r="G151" s="27"/>
       <c r="H151" s="27"/>
-      <c r="I151" s="346"/>
-      <c r="J151" s="346"/>
+      <c r="I151" s="338"/>
+      <c r="J151" s="338"/>
       <c r="K151" s="27"/>
       <c r="L151" s="27"/>
       <c r="M151" s="34"/>
@@ -45990,8 +46531,8 @@
       <c r="F152" s="27"/>
       <c r="G152" s="27"/>
       <c r="H152" s="27"/>
-      <c r="I152" s="346"/>
-      <c r="J152" s="346"/>
+      <c r="I152" s="338"/>
+      <c r="J152" s="338"/>
       <c r="K152" s="27"/>
       <c r="L152" s="27"/>
       <c r="M152" s="34"/>
@@ -46007,8 +46548,8 @@
       <c r="H153" s="31" t="s">
         <v>3248</v>
       </c>
-      <c r="I153" s="346"/>
-      <c r="J153" s="346"/>
+      <c r="I153" s="338"/>
+      <c r="J153" s="338"/>
       <c r="K153" s="27"/>
       <c r="L153" s="27"/>
       <c r="M153" s="34"/>
@@ -46025,8 +46566,8 @@
       <c r="H154" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="I154" s="346"/>
-      <c r="J154" s="346"/>
+      <c r="I154" s="338"/>
+      <c r="J154" s="338"/>
       <c r="K154" s="27"/>
       <c r="L154" s="27"/>
       <c r="M154" s="34"/>
@@ -46040,8 +46581,8 @@
       <c r="H155" s="27">
         <v>20</v>
       </c>
-      <c r="I155" s="346"/>
-      <c r="J155" s="346"/>
+      <c r="I155" s="338"/>
+      <c r="J155" s="338"/>
       <c r="K155" s="27"/>
       <c r="L155" s="27"/>
       <c r="M155" s="34"/>
@@ -46055,8 +46596,8 @@
       <c r="H156" s="36" t="s">
         <v>3241</v>
       </c>
-      <c r="I156" s="346"/>
-      <c r="J156" s="346"/>
+      <c r="I156" s="338"/>
+      <c r="J156" s="338"/>
       <c r="K156" s="27"/>
       <c r="L156" s="27"/>
       <c r="M156" s="34"/>
@@ -46066,8 +46607,8 @@
       <c r="F157" s="27"/>
       <c r="G157" s="27"/>
       <c r="H157" s="27"/>
-      <c r="I157" s="346"/>
-      <c r="J157" s="346"/>
+      <c r="I157" s="338"/>
+      <c r="J157" s="338"/>
       <c r="K157" s="27"/>
       <c r="L157" s="27"/>
       <c r="M157" s="34"/>
@@ -46083,8 +46624,8 @@
       <c r="H158" s="31" t="s">
         <v>3248</v>
       </c>
-      <c r="I158" s="346"/>
-      <c r="J158" s="346"/>
+      <c r="I158" s="338"/>
+      <c r="J158" s="338"/>
       <c r="K158" s="27"/>
       <c r="L158" s="27"/>
       <c r="M158" s="34"/>
@@ -46098,8 +46639,8 @@
       <c r="H159" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="I159" s="346"/>
-      <c r="J159" s="346"/>
+      <c r="I159" s="338"/>
+      <c r="J159" s="338"/>
       <c r="K159" s="27"/>
       <c r="L159" s="27"/>
       <c r="M159" s="34"/>
@@ -46113,8 +46654,8 @@
       <c r="H160" s="27">
         <v>18</v>
       </c>
-      <c r="I160" s="346"/>
-      <c r="J160" s="346"/>
+      <c r="I160" s="338"/>
+      <c r="J160" s="338"/>
       <c r="K160" s="27"/>
       <c r="L160" s="27"/>
       <c r="M160" s="34"/>
@@ -46128,8 +46669,8 @@
       <c r="H161" s="36" t="s">
         <v>3242</v>
       </c>
-      <c r="I161" s="347"/>
-      <c r="J161" s="347"/>
+      <c r="I161" s="339"/>
+      <c r="J161" s="339"/>
       <c r="K161" s="27"/>
       <c r="L161" s="27"/>
       <c r="M161" s="34"/>
@@ -51110,10 +51651,375 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M33"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:13">
+      <c r="B2" s="350" t="s">
+        <v>2552</v>
+      </c>
+      <c r="C2" s="351"/>
+      <c r="D2" s="352"/>
+      <c r="F2" s="350" t="s">
+        <v>3251</v>
+      </c>
+      <c r="G2" s="351"/>
+      <c r="H2" s="351"/>
+      <c r="I2" s="352"/>
+      <c r="K2" s="350" t="s">
+        <v>3253</v>
+      </c>
+      <c r="L2" s="351"/>
+      <c r="M2" s="352"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" s="353"/>
+      <c r="C3" s="354"/>
+      <c r="D3" s="355"/>
+      <c r="F3" s="353"/>
+      <c r="G3" s="354"/>
+      <c r="H3" s="354"/>
+      <c r="I3" s="355"/>
+      <c r="K3" s="353"/>
+      <c r="L3" s="354"/>
+      <c r="M3" s="355"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" s="353"/>
+      <c r="C4" s="354"/>
+      <c r="D4" s="355"/>
+      <c r="F4" s="353"/>
+      <c r="G4" s="354"/>
+      <c r="H4" s="354"/>
+      <c r="I4" s="355"/>
+      <c r="K4" s="353"/>
+      <c r="L4" s="354"/>
+      <c r="M4" s="355"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="356" t="s">
+        <v>2337</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="41">
+        <v>100000</v>
+      </c>
+      <c r="F5" s="80"/>
+      <c r="G5" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>524</v>
+      </c>
+      <c r="I5" s="41"/>
+      <c r="K5" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>559</v>
+      </c>
+      <c r="M5" s="41"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="356"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>412</v>
+      </c>
+      <c r="F6" s="80"/>
+      <c r="G6" s="39" t="s">
+        <v>3222</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>3252</v>
+      </c>
+      <c r="I6" s="41"/>
+      <c r="K6" s="80" t="s">
+        <v>3222</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>3254</v>
+      </c>
+      <c r="M6" s="41"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="356"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="39" t="s">
+        <v>3255</v>
+      </c>
+      <c r="D7" s="41">
+        <v>750</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="34"/>
+      <c r="K7" s="80" t="s">
+        <v>3264</v>
+      </c>
+      <c r="L7" s="39">
+        <v>50000</v>
+      </c>
+      <c r="M7" s="41"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="33"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="34"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="34"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="356" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="348" t="s">
+        <v>3250</v>
+      </c>
+      <c r="C9" s="143"/>
+      <c r="D9" s="258"/>
+      <c r="F9" s="348" t="s">
+        <v>3258</v>
+      </c>
+      <c r="G9" s="143"/>
+      <c r="H9" s="143"/>
+      <c r="I9" s="258"/>
+      <c r="K9" s="348" t="s">
+        <v>3257</v>
+      </c>
+      <c r="L9" s="143"/>
+      <c r="M9" s="258"/>
+    </row>
+    <row r="10" spans="1:13" ht="30.75" customHeight="1">
+      <c r="A10" s="356"/>
+      <c r="B10" s="348"/>
+      <c r="C10" s="349" t="s">
+        <v>3260</v>
+      </c>
+      <c r="D10" s="258"/>
+      <c r="E10" t="s">
+        <v>3262</v>
+      </c>
+      <c r="F10" s="348"/>
+      <c r="G10" s="143" t="s">
+        <v>3263</v>
+      </c>
+      <c r="H10" s="258"/>
+      <c r="I10" s="258"/>
+      <c r="K10" s="348"/>
+      <c r="L10" s="143" t="s">
+        <v>3256</v>
+      </c>
+      <c r="M10" s="258"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="356"/>
+      <c r="B11" s="348"/>
+      <c r="C11" s="143"/>
+      <c r="D11" s="258"/>
+      <c r="F11" s="348"/>
+      <c r="G11" s="143"/>
+      <c r="H11" s="258" t="s">
+        <v>3259</v>
+      </c>
+      <c r="I11" s="258"/>
+      <c r="J11" t="s">
+        <v>3261</v>
+      </c>
+      <c r="K11" s="348"/>
+      <c r="L11" s="143"/>
+      <c r="M11" s="258" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="356"/>
+      <c r="B12" s="348"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="258"/>
+      <c r="F12" s="348"/>
+      <c r="G12" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="258"/>
+      <c r="I12" s="258"/>
+      <c r="K12" s="348"/>
+      <c r="L12" s="143" t="s">
+        <v>137</v>
+      </c>
+      <c r="M12" s="258"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="33"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="34"/>
+      <c r="F13" s="348"/>
+      <c r="G13" s="143"/>
+      <c r="H13" s="258" t="s">
+        <v>2210</v>
+      </c>
+      <c r="I13" s="258"/>
+      <c r="K13" s="348"/>
+      <c r="L13" s="143"/>
+      <c r="M13" s="258" t="s">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="87"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>3265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="B17" t="s">
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="B18" t="s">
+        <v>3267</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3271</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="H19" t="s">
+        <v>3273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>3268</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" t="s">
+        <v>3269</v>
+      </c>
+      <c r="H21" t="s">
+        <v>3275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="B22" t="s">
+        <v>3270</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1">
+      <c r="D24" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" s="43"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="34"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B27" s="43"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="34"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B28" s="43"/>
+      <c r="D28" s="357"/>
+      <c r="E28" s="358"/>
+      <c r="F28" s="359"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B29" s="43"/>
+      <c r="D29" s="357"/>
+      <c r="E29" s="358"/>
+      <c r="F29" s="359"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B30" s="43"/>
+      <c r="D30" s="357"/>
+      <c r="E30" s="358"/>
+      <c r="F30" s="359"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="43"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="D32" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:D4"/>
+    <mergeCell ref="F2:I4"/>
+    <mergeCell ref="K2:M4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A9:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R411"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P53" sqref="P53"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -51131,23 +52037,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="335" t="s">
+      <c r="A1" s="341" t="s">
         <v>2815</v>
       </c>
-      <c r="B1" s="335"/>
-      <c r="C1" s="335"/>
-      <c r="D1" s="335"/>
-      <c r="E1" s="335"/>
-      <c r="F1" s="335"/>
-      <c r="I1" s="335" t="s">
+      <c r="B1" s="341"/>
+      <c r="C1" s="341"/>
+      <c r="D1" s="341"/>
+      <c r="E1" s="341"/>
+      <c r="F1" s="341"/>
+      <c r="I1" s="341" t="s">
         <v>2827</v>
       </c>
-      <c r="J1" s="335"/>
-      <c r="K1" s="335"/>
-      <c r="L1" s="335"/>
-      <c r="M1" s="335"/>
-      <c r="N1" s="335"/>
-      <c r="O1" s="335"/>
+      <c r="J1" s="341"/>
+      <c r="K1" s="341"/>
+      <c r="L1" s="341"/>
+      <c r="M1" s="341"/>
+      <c r="N1" s="341"/>
+      <c r="O1" s="341"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -51306,24 +52212,24 @@
       <c r="A12" s="328" t="s">
         <v>2829</v>
       </c>
-      <c r="B12" s="334"/>
-      <c r="C12" s="334"/>
-      <c r="D12" s="334"/>
-      <c r="E12" s="334"/>
-      <c r="F12" s="334"/>
-      <c r="G12" s="334"/>
+      <c r="B12" s="340"/>
+      <c r="C12" s="340"/>
+      <c r="D12" s="340"/>
+      <c r="E12" s="340"/>
+      <c r="F12" s="340"/>
+      <c r="G12" s="340"/>
       <c r="H12" s="329"/>
       <c r="I12" s="328" t="s">
         <v>2829</v>
       </c>
-      <c r="J12" s="334"/>
-      <c r="K12" s="334"/>
-      <c r="L12" s="334"/>
-      <c r="M12" s="334"/>
-      <c r="N12" s="334"/>
-      <c r="O12" s="334"/>
-      <c r="P12" s="334"/>
-      <c r="Q12" s="334"/>
+      <c r="J12" s="340"/>
+      <c r="K12" s="340"/>
+      <c r="L12" s="340"/>
+      <c r="M12" s="340"/>
+      <c r="N12" s="340"/>
+      <c r="O12" s="340"/>
+      <c r="P12" s="340"/>
+      <c r="Q12" s="340"/>
       <c r="R12" s="329"/>
     </row>
     <row r="13" spans="1:18">
@@ -51552,14 +52458,14 @@
       <c r="R21" s="37"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="335" t="s">
+      <c r="A24" s="341" t="s">
         <v>2815</v>
       </c>
-      <c r="B24" s="335"/>
-      <c r="C24" s="335"/>
-      <c r="D24" s="335"/>
-      <c r="E24" s="335"/>
-      <c r="F24" s="335"/>
+      <c r="B24" s="341"/>
+      <c r="C24" s="341"/>
+      <c r="D24" s="341"/>
+      <c r="E24" s="341"/>
+      <c r="F24" s="341"/>
       <c r="H24" s="272" t="s">
         <v>2827</v>
       </c>
@@ -51569,11 +52475,11 @@
       <c r="L24" s="272"/>
       <c r="M24" s="272"/>
       <c r="N24" s="272"/>
-      <c r="P24" s="335" t="s">
+      <c r="P24" s="341" t="s">
         <v>2868</v>
       </c>
-      <c r="Q24" s="335"/>
-      <c r="R24" s="335"/>
+      <c r="Q24" s="341"/>
+      <c r="R24" s="341"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="106" t="s">
@@ -51816,24 +52722,24 @@
       <c r="A35" s="328" t="s">
         <v>2869</v>
       </c>
-      <c r="B35" s="334"/>
-      <c r="C35" s="334"/>
-      <c r="D35" s="334"/>
-      <c r="E35" s="334"/>
-      <c r="F35" s="334"/>
-      <c r="G35" s="334"/>
+      <c r="B35" s="340"/>
+      <c r="C35" s="340"/>
+      <c r="D35" s="340"/>
+      <c r="E35" s="340"/>
+      <c r="F35" s="340"/>
+      <c r="G35" s="340"/>
       <c r="H35" s="329"/>
       <c r="I35" s="328" t="s">
         <v>1131</v>
       </c>
-      <c r="J35" s="334"/>
-      <c r="K35" s="334"/>
-      <c r="L35" s="334"/>
-      <c r="M35" s="334"/>
-      <c r="N35" s="334"/>
-      <c r="O35" s="334"/>
-      <c r="P35" s="334"/>
-      <c r="Q35" s="334"/>
+      <c r="J35" s="340"/>
+      <c r="K35" s="340"/>
+      <c r="L35" s="340"/>
+      <c r="M35" s="340"/>
+      <c r="N35" s="340"/>
+      <c r="O35" s="340"/>
+      <c r="P35" s="340"/>
+      <c r="Q35" s="340"/>
       <c r="R35" s="329"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" thickBot="1">
@@ -55375,437 +56281,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D3:H121"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="3" spans="4:6">
-      <c r="D3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="4" spans="4:6">
-      <c r="D4" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="6" spans="4:6">
-      <c r="D6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="4:6">
-      <c r="E7" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="8" spans="4:6">
-      <c r="E8" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="10" spans="4:6">
-      <c r="E10" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="11" spans="4:6">
-      <c r="F11" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="12" spans="4:6">
-      <c r="E12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="4:6">
-      <c r="D13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="4:6">
-      <c r="D14" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6">
-      <c r="D15" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5">
-      <c r="D18" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5">
-      <c r="D20" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5">
-      <c r="E21" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5">
-      <c r="E22" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5">
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5">
-      <c r="D25" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="27" spans="4:5">
-      <c r="D27" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="28" spans="4:5">
-      <c r="E28" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="29" spans="4:5">
-      <c r="E29" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5">
-      <c r="E31" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5">
-      <c r="D32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="4:5">
-      <c r="D35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="4:5">
-      <c r="D36" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="37" spans="4:5">
-      <c r="D37" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="38" spans="4:5">
-      <c r="D38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="4:5">
-      <c r="D39" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="40" spans="4:5">
-      <c r="E40" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="41" spans="4:5">
-      <c r="D41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5">
-      <c r="D42" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="43" spans="4:5">
-      <c r="D43" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5">
-      <c r="D44" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="45" spans="4:5">
-      <c r="D45" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="46" spans="4:5">
-      <c r="E46" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="47" spans="4:5">
-      <c r="D47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="4:5">
-      <c r="D48" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="51" spans="4:8">
-      <c r="D51" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="52" spans="4:8">
-      <c r="E52" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="53" spans="4:8">
-      <c r="F53" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="54" spans="4:8">
-      <c r="G54" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="56" spans="4:8">
-      <c r="G56" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="57" spans="4:8">
-      <c r="G57" t="s">
-        <v>371</v>
-      </c>
-      <c r="H57" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="58" spans="4:8">
-      <c r="G58" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="60" spans="4:8">
-      <c r="G60" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="62" spans="4:8">
-      <c r="G62" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="63" spans="4:8">
-      <c r="F63" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="64" spans="4:8">
-      <c r="E64" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="4:7">
-      <c r="D66" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="4:7">
-      <c r="D68" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="69" spans="4:7">
-      <c r="D69" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="70" spans="4:7">
-      <c r="D70" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="75" spans="4:7">
-      <c r="D75" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="76" spans="4:7">
-      <c r="E76" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="77" spans="4:7">
-      <c r="E77" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="78" spans="4:7">
-      <c r="F78" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="79" spans="4:7">
-      <c r="G79" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="80" spans="4:7">
-      <c r="F80" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="81" spans="4:5">
-      <c r="E81" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="82" spans="4:5">
-      <c r="D82" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="83" spans="4:5">
-      <c r="D83" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="88" spans="4:5">
-      <c r="D88" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="91" spans="4:5">
-      <c r="D91" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="92" spans="4:5">
-      <c r="D92" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="93" spans="4:5">
-      <c r="D93" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="96" spans="4:5">
-      <c r="D96" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="101" spans="4:5">
-      <c r="D101" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="102" spans="4:5">
-      <c r="E102" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="103" spans="4:5">
-      <c r="D103" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="104" spans="4:5">
-      <c r="E104" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="105" spans="4:5">
-      <c r="D105" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="106" spans="4:5">
-      <c r="E106" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="107" spans="4:5">
-      <c r="E107" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="108" spans="4:5">
-      <c r="E108" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="111" spans="4:5">
-      <c r="E111" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="112" spans="4:5">
-      <c r="D112" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="113" spans="4:6">
-      <c r="E113" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="114" spans="4:6">
-      <c r="E114" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="115" spans="4:6">
-      <c r="F115" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="116" spans="4:6">
-      <c r="F116" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="117" spans="4:6">
-      <c r="F117" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="119" spans="4:6">
-      <c r="F119" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="120" spans="4:6">
-      <c r="E120" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="121" spans="4:6">
-      <c r="D121" t="s">
-        <v>144</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
abstract, access and polymorphism
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="10" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="pc-basics" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5915" uniqueCount="3151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5921" uniqueCount="3153">
   <si>
     <t>USER</t>
   </si>
@@ -9739,6 +9739,12 @@
   </si>
   <si>
     <t>Confused</t>
+  </si>
+  <si>
+    <t>((IphoneX) i3) . faceRecog();</t>
+  </si>
+  <si>
+    <t>Typecasting</t>
   </si>
 </sst>
 </file>
@@ -9835,13 +9841,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -9868,8 +9867,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9993,6 +9999,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10353,12 +10365,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="370">
+  <cellXfs count="373">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -10930,7 +10942,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -10950,7 +10961,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10998,10 +11009,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11114,13 +11132,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11454,13 +11469,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1">
-      <c r="H3" s="336" t="s">
+      <c r="H3" s="338" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="337"/>
-      <c r="J3" s="337"/>
-      <c r="K3" s="337"/>
-      <c r="L3" s="338"/>
+      <c r="I3" s="339"/>
+      <c r="J3" s="339"/>
+      <c r="K3" s="339"/>
+      <c r="L3" s="340"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:18" ht="15.75" thickBot="1">
@@ -11481,20 +11496,20 @@
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1">
       <c r="F6" s="4"/>
-      <c r="G6" s="339" t="s">
+      <c r="G6" s="341" t="s">
         <v>1572</v>
       </c>
-      <c r="H6" s="340"/>
+      <c r="H6" s="342"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="339" t="s">
+      <c r="J6" s="341" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="340"/>
+      <c r="K6" s="342"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="339" t="s">
+      <c r="M6" s="341" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="340"/>
+      <c r="N6" s="342"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1">
       <c r="D7" s="125" t="s">
@@ -11512,20 +11527,20 @@
     </row>
     <row r="8" spans="1:18">
       <c r="F8" s="4"/>
-      <c r="G8" s="341" t="s">
+      <c r="G8" s="343" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="342"/>
+      <c r="H8" s="344"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="341" t="s">
+      <c r="J8" s="343" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="342"/>
+      <c r="K8" s="344"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="341" t="s">
+      <c r="M8" s="343" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="342"/>
+      <c r="N8" s="344"/>
       <c r="Q8" s="142"/>
     </row>
     <row r="9" spans="1:18">
@@ -11541,29 +11556,29 @@
       <c r="Q9" s="142"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="F10" s="332" t="s">
+      <c r="F10" s="334" t="s">
         <v>2505</v>
       </c>
-      <c r="G10" s="333"/>
-      <c r="H10" s="333"/>
-      <c r="I10" s="333"/>
-      <c r="J10" s="333"/>
-      <c r="K10" s="333"/>
-      <c r="L10" s="333"/>
-      <c r="M10" s="333"/>
-      <c r="N10" s="333"/>
+      <c r="G10" s="335"/>
+      <c r="H10" s="335"/>
+      <c r="I10" s="335"/>
+      <c r="J10" s="335"/>
+      <c r="K10" s="335"/>
+      <c r="L10" s="335"/>
+      <c r="M10" s="335"/>
+      <c r="N10" s="335"/>
       <c r="Q10" s="142"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1">
-      <c r="F11" s="334"/>
-      <c r="G11" s="335"/>
-      <c r="H11" s="335"/>
-      <c r="I11" s="335"/>
-      <c r="J11" s="335"/>
-      <c r="K11" s="335"/>
-      <c r="L11" s="335"/>
-      <c r="M11" s="335"/>
-      <c r="N11" s="335"/>
+      <c r="F11" s="336"/>
+      <c r="G11" s="337"/>
+      <c r="H11" s="337"/>
+      <c r="I11" s="337"/>
+      <c r="J11" s="337"/>
+      <c r="K11" s="337"/>
+      <c r="L11" s="337"/>
+      <c r="M11" s="337"/>
+      <c r="N11" s="337"/>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
@@ -11605,17 +11620,17 @@
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1">
       <c r="D14" s="125"/>
-      <c r="F14" s="329" t="s">
+      <c r="F14" s="331" t="s">
         <v>2920</v>
       </c>
-      <c r="G14" s="330"/>
-      <c r="H14" s="330"/>
-      <c r="I14" s="330"/>
-      <c r="J14" s="330"/>
-      <c r="K14" s="330"/>
-      <c r="L14" s="330"/>
-      <c r="M14" s="330"/>
-      <c r="N14" s="331"/>
+      <c r="G14" s="332"/>
+      <c r="H14" s="332"/>
+      <c r="I14" s="332"/>
+      <c r="J14" s="332"/>
+      <c r="K14" s="332"/>
+      <c r="L14" s="332"/>
+      <c r="M14" s="332"/>
+      <c r="N14" s="333"/>
     </row>
     <row r="15" spans="1:18">
       <c r="F15" s="139"/>
@@ -11918,7 +11933,7 @@
       <c r="D33" s="74"/>
       <c r="E33" s="74"/>
       <c r="F33" s="74"/>
-      <c r="G33" s="304" t="s">
+      <c r="G33" s="303" t="s">
         <v>2940</v>
       </c>
       <c r="H33" s="132" t="s">
@@ -11951,28 +11966,28 @@
       <c r="G34" s="145">
         <v>0</v>
       </c>
-      <c r="H34" s="305">
+      <c r="H34" s="304">
         <v>1</v>
       </c>
-      <c r="I34" s="305">
+      <c r="I34" s="304">
         <v>1</v>
       </c>
-      <c r="J34" s="305">
+      <c r="J34" s="304">
         <v>1</v>
       </c>
-      <c r="K34" s="305">
+      <c r="K34" s="304">
         <v>1</v>
       </c>
-      <c r="L34" s="305">
+      <c r="L34" s="304">
         <v>1</v>
       </c>
-      <c r="M34" s="305">
+      <c r="M34" s="304">
         <v>1</v>
       </c>
-      <c r="N34" s="305">
+      <c r="N34" s="304">
         <v>1</v>
       </c>
-      <c r="P34" s="303" t="s">
+      <c r="P34" s="302" t="s">
         <v>2976</v>
       </c>
     </row>
@@ -18752,7 +18767,7 @@
       <c r="H32" t="s">
         <v>3113</v>
       </c>
-      <c r="I32" s="328" t="s">
+      <c r="I32" s="327" t="s">
         <v>3119</v>
       </c>
     </row>
@@ -19564,10 +19579,10 @@
       <c r="J5" s="158" t="s">
         <v>2283</v>
       </c>
-      <c r="K5" s="368" t="s">
+      <c r="K5" s="329" t="s">
         <v>3134</v>
       </c>
-      <c r="L5" s="369"/>
+      <c r="L5" s="330"/>
       <c r="N5" s="34"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1">
@@ -19617,10 +19632,10 @@
       <c r="J9" s="158" t="s">
         <v>2283</v>
       </c>
-      <c r="K9" s="368" t="s">
+      <c r="K9" s="329" t="s">
         <v>3135</v>
       </c>
-      <c r="L9" s="369"/>
+      <c r="L9" s="330"/>
       <c r="N9" s="34"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1">
@@ -19669,10 +19684,10 @@
       <c r="J13" s="158" t="s">
         <v>2283</v>
       </c>
-      <c r="K13" s="368" t="s">
+      <c r="K13" s="329" t="s">
         <v>3135</v>
       </c>
-      <c r="L13" s="369"/>
+      <c r="L13" s="330"/>
       <c r="N13" s="34"/>
     </row>
     <row r="14" spans="1:14">
@@ -20096,7 +20111,7 @@
       <c r="H224" s="38"/>
     </row>
     <row r="229" spans="1:3">
-      <c r="A229" s="367"/>
+      <c r="A229" s="328"/>
       <c r="B229" s="39"/>
       <c r="C229" s="39"/>
     </row>
@@ -20110,7 +20125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -20338,13 +20353,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:V272"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G81" sqref="G81"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:18">
       <c r="H2" t="s">
         <v>2717</v>
       </c>
@@ -20355,25 +20370,34 @@
         <v>743</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:18">
       <c r="H4" t="s">
         <v>2719</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:18">
       <c r="H5" t="s">
         <v>2720</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:18">
       <c r="H6" s="56" t="s">
         <v>2721</v>
       </c>
       <c r="I6" s="56"/>
       <c r="J6" s="56"/>
     </row>
-    <row r="8" spans="2:13" ht="15.75" thickBot="1"/>
-    <row r="9" spans="2:13">
+    <row r="7" spans="2:18">
+      <c r="Q7" t="s">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="15.75" thickBot="1">
+      <c r="Q8" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18">
       <c r="B9" s="284"/>
       <c r="C9" s="285"/>
       <c r="D9" s="286"/>
@@ -20382,13 +20406,18 @@
         <v>2716</v>
       </c>
       <c r="H9" s="32"/>
-      <c r="K9" s="284"/>
-      <c r="L9" s="287" t="s">
+      <c r="K9" s="370"/>
+      <c r="L9" s="371" t="s">
         <v>2716</v>
       </c>
-      <c r="M9" s="286"/>
-    </row>
-    <row r="10" spans="2:13">
+      <c r="M9" s="372"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="369" t="s">
+        <v>2716</v>
+      </c>
+      <c r="R9" s="83"/>
+    </row>
+    <row r="10" spans="2:18">
       <c r="B10" s="33"/>
       <c r="C10" s="27"/>
       <c r="D10" s="34"/>
@@ -20398,8 +20427,11 @@
       <c r="K10" s="33"/>
       <c r="L10" s="27"/>
       <c r="M10" s="34"/>
-    </row>
-    <row r="11" spans="2:13">
+      <c r="P10" s="33"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="34"/>
+    </row>
+    <row r="11" spans="2:18">
       <c r="B11" s="33"/>
       <c r="C11" s="27"/>
       <c r="D11" s="34"/>
@@ -20409,8 +20441,11 @@
       <c r="K11" s="33"/>
       <c r="L11" s="27"/>
       <c r="M11" s="34"/>
-    </row>
-    <row r="12" spans="2:13">
+      <c r="P11" s="33"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="34"/>
+    </row>
+    <row r="12" spans="2:18">
       <c r="B12" s="33"/>
       <c r="C12" s="27"/>
       <c r="D12" s="34"/>
@@ -20420,8 +20455,11 @@
       <c r="K12" s="33"/>
       <c r="L12" s="27"/>
       <c r="M12" s="34"/>
-    </row>
-    <row r="13" spans="2:13">
+      <c r="P12" s="33"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="34"/>
+    </row>
+    <row r="13" spans="2:18">
       <c r="B13" s="33"/>
       <c r="C13" s="27"/>
       <c r="D13" s="34"/>
@@ -20437,8 +20475,11 @@
       <c r="K13" s="33"/>
       <c r="L13" s="27"/>
       <c r="M13" s="34"/>
-    </row>
-    <row r="14" spans="2:13">
+      <c r="P13" s="33"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="34"/>
+    </row>
+    <row r="14" spans="2:18">
       <c r="B14" s="33" t="s">
         <v>2722</v>
       </c>
@@ -20460,8 +20501,15 @@
       <c r="M14" s="34" t="s">
         <v>2723</v>
       </c>
-    </row>
-    <row r="15" spans="2:13">
+      <c r="P14" s="33" t="s">
+        <v>2722</v>
+      </c>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="34" t="s">
+        <v>2723</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18">
       <c r="B15" s="33"/>
       <c r="C15" s="27"/>
       <c r="D15" s="34"/>
@@ -20471,8 +20519,11 @@
       <c r="K15" s="33"/>
       <c r="L15" s="27"/>
       <c r="M15" s="34"/>
-    </row>
-    <row r="16" spans="2:13">
+      <c r="P15" s="33"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="34"/>
+    </row>
+    <row r="16" spans="2:18">
       <c r="B16" s="33"/>
       <c r="C16" s="27" t="s">
         <v>2724</v>
@@ -20488,8 +20539,13 @@
         <v>2724</v>
       </c>
       <c r="M16" s="34"/>
-    </row>
-    <row r="17" spans="2:13">
+      <c r="P16" s="33"/>
+      <c r="Q16" s="27" t="s">
+        <v>2724</v>
+      </c>
+      <c r="R16" s="34"/>
+    </row>
+    <row r="17" spans="2:18">
       <c r="B17" s="278"/>
       <c r="C17" s="279"/>
       <c r="D17" s="280"/>
@@ -20499,8 +20555,11 @@
       <c r="K17" s="278"/>
       <c r="L17" s="279"/>
       <c r="M17" s="280"/>
-    </row>
-    <row r="18" spans="2:13" ht="15.75" thickBot="1">
+      <c r="P17" s="278"/>
+      <c r="Q17" s="279"/>
+      <c r="R17" s="280"/>
+    </row>
+    <row r="18" spans="2:18" ht="15.75" thickBot="1">
       <c r="B18" s="281"/>
       <c r="C18" s="282"/>
       <c r="D18" s="283"/>
@@ -20510,10 +20569,13 @@
       <c r="K18" s="281"/>
       <c r="L18" s="282"/>
       <c r="M18" s="283"/>
-    </row>
-    <row r="19" spans="2:13">
+      <c r="P18" s="281"/>
+      <c r="Q18" s="282"/>
+      <c r="R18" s="283"/>
+    </row>
+    <row r="19" spans="2:18">
       <c r="C19" t="s">
-        <v>1489</v>
+        <v>744</v>
       </c>
       <c r="G19" t="s">
         <v>743</v>
@@ -24705,7 +24767,7 @@
       </c>
       <c r="L3" s="47"/>
       <c r="M3" s="48"/>
-      <c r="N3" s="361" t="s">
+      <c r="N3" s="363" t="s">
         <v>2753</v>
       </c>
       <c r="O3" s="51"/>
@@ -24734,7 +24796,7 @@
       <c r="K4" s="51"/>
       <c r="L4" s="50"/>
       <c r="M4" s="51"/>
-      <c r="N4" s="346"/>
+      <c r="N4" s="348"/>
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
       <c r="Q4" s="52"/>
@@ -24760,7 +24822,7 @@
       <c r="M5" s="51" t="s">
         <v>559</v>
       </c>
-      <c r="N5" s="346"/>
+      <c r="N5" s="348"/>
       <c r="O5" s="51"/>
       <c r="P5" s="51"/>
       <c r="Q5" s="52"/>
@@ -24782,7 +24844,7 @@
       <c r="M6" s="54">
         <v>12345</v>
       </c>
-      <c r="N6" s="346"/>
+      <c r="N6" s="348"/>
       <c r="O6" s="51"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="52"/>
@@ -24800,7 +24862,7 @@
       <c r="K7" s="51"/>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
-      <c r="N7" s="346"/>
+      <c r="N7" s="348"/>
       <c r="O7" s="51"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="52"/>
@@ -24820,7 +24882,7 @@
       </c>
       <c r="L8" s="47"/>
       <c r="M8" s="48"/>
-      <c r="N8" s="346"/>
+      <c r="N8" s="348"/>
       <c r="O8" s="51"/>
       <c r="P8" s="51"/>
       <c r="Q8" s="52"/>
@@ -24838,7 +24900,7 @@
       <c r="K9" s="51"/>
       <c r="L9" s="50"/>
       <c r="M9" s="51"/>
-      <c r="N9" s="346"/>
+      <c r="N9" s="348"/>
       <c r="O9" s="51"/>
       <c r="P9" s="51"/>
       <c r="Q9" s="52"/>
@@ -24855,7 +24917,7 @@
       <c r="M10" s="51" t="s">
         <v>524</v>
       </c>
-      <c r="N10" s="346"/>
+      <c r="N10" s="348"/>
       <c r="O10" s="51"/>
       <c r="P10" s="51"/>
       <c r="Q10" s="52"/>
@@ -24875,7 +24937,7 @@
       <c r="M11" s="54">
         <v>12346</v>
       </c>
-      <c r="N11" s="347"/>
+      <c r="N11" s="349"/>
       <c r="O11" s="51"/>
       <c r="P11" s="51"/>
       <c r="Q11" s="52"/>
@@ -28005,7 +28067,7 @@
       <c r="N284" s="49">
         <v>10</v>
       </c>
-      <c r="O284" s="288" t="s">
+      <c r="O284" s="287" t="s">
         <v>2488</v>
       </c>
       <c r="P284" s="51"/>
@@ -28030,7 +28092,7 @@
       <c r="L285" s="51"/>
       <c r="M285" s="53"/>
       <c r="N285" s="55"/>
-      <c r="O285" s="288"/>
+      <c r="O285" s="287"/>
       <c r="P285" s="51"/>
       <c r="Q285" s="52"/>
     </row>
@@ -28053,7 +28115,7 @@
       <c r="L286" s="51"/>
       <c r="M286" s="51"/>
       <c r="N286" s="51"/>
-      <c r="O286" s="288"/>
+      <c r="O286" s="287"/>
       <c r="P286" s="51"/>
       <c r="Q286" s="52"/>
     </row>
@@ -28076,7 +28138,7 @@
       <c r="N287" s="49">
         <v>10</v>
       </c>
-      <c r="O287" s="288"/>
+      <c r="O287" s="287"/>
       <c r="P287" s="51"/>
       <c r="Q287" s="52"/>
     </row>
@@ -28093,7 +28155,7 @@
       <c r="L288" s="51"/>
       <c r="M288" s="53"/>
       <c r="N288" s="55"/>
-      <c r="O288" s="288"/>
+      <c r="O288" s="287"/>
       <c r="P288" s="51"/>
       <c r="Q288" s="52"/>
     </row>
@@ -28112,7 +28174,7 @@
       <c r="L289" s="51"/>
       <c r="M289" s="51"/>
       <c r="N289" s="51"/>
-      <c r="O289" s="288"/>
+      <c r="O289" s="287"/>
       <c r="P289" s="51"/>
       <c r="Q289" s="52"/>
     </row>
@@ -28137,7 +28199,7 @@
       <c r="N290" s="49">
         <v>10</v>
       </c>
-      <c r="O290" s="288"/>
+      <c r="O290" s="287"/>
       <c r="P290" s="51"/>
       <c r="Q290" s="52"/>
     </row>
@@ -28156,7 +28218,7 @@
       <c r="L291" s="51"/>
       <c r="M291" s="53"/>
       <c r="N291" s="55"/>
-      <c r="O291" s="288"/>
+      <c r="O291" s="287"/>
       <c r="P291" s="51"/>
       <c r="Q291" s="52"/>
     </row>
@@ -28299,7 +28361,7 @@
       <c r="G6" s="33" t="s">
         <v>2765</v>
       </c>
-      <c r="H6" s="289">
+      <c r="H6" s="288">
         <v>0</v>
       </c>
       <c r="I6" s="27" t="s">
@@ -28315,7 +28377,7 @@
         <v>2761</v>
       </c>
       <c r="G7" s="33"/>
-      <c r="H7" s="289">
+      <c r="H7" s="288">
         <v>1</v>
       </c>
       <c r="I7" s="27" t="s">
@@ -28336,7 +28398,7 @@
         <v>2774</v>
       </c>
       <c r="G8" s="33"/>
-      <c r="H8" s="289">
+      <c r="H8" s="288">
         <v>2</v>
       </c>
       <c r="I8" s="27" t="s">
@@ -28356,7 +28418,7 @@
         <v>2769</v>
       </c>
       <c r="G9" s="33"/>
-      <c r="H9" s="289">
+      <c r="H9" s="288">
         <v>3</v>
       </c>
       <c r="I9" s="27" t="s">
@@ -28372,7 +28434,7 @@
         <v>2770</v>
       </c>
       <c r="G10" s="33"/>
-      <c r="H10" s="289">
+      <c r="H10" s="288">
         <v>4</v>
       </c>
       <c r="I10" s="27" t="s">
@@ -28491,14 +28553,14 @@
       <c r="E24" s="57">
         <v>0</v>
       </c>
-      <c r="F24" s="289"/>
-      <c r="G24" s="289"/>
+      <c r="F24" s="288"/>
+      <c r="G24" s="288"/>
     </row>
     <row r="25" spans="1:13">
       <c r="E25" s="57">
         <v>1</v>
       </c>
-      <c r="F25" s="289"/>
+      <c r="F25" s="288"/>
       <c r="G25" s="132">
         <v>234</v>
       </c>
@@ -28507,15 +28569,15 @@
       <c r="E26" s="57">
         <v>2</v>
       </c>
-      <c r="F26" s="289"/>
-      <c r="G26" s="289"/>
+      <c r="F26" s="288"/>
+      <c r="G26" s="288"/>
     </row>
     <row r="27" spans="1:13">
       <c r="E27" s="57">
         <v>3</v>
       </c>
-      <c r="F27" s="289"/>
-      <c r="G27" s="289"/>
+      <c r="F27" s="288"/>
+      <c r="G27" s="288"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
@@ -28527,7 +28589,7 @@
       <c r="E29" s="129">
         <v>0</v>
       </c>
-      <c r="F29" s="289">
+      <c r="F29" s="288">
         <v>10</v>
       </c>
       <c r="H29" t="s">
@@ -28536,7 +28598,7 @@
       <c r="I29" s="129">
         <v>0</v>
       </c>
-      <c r="J29" s="289">
+      <c r="J29" s="288">
         <v>0</v>
       </c>
     </row>
@@ -28547,13 +28609,13 @@
       <c r="E30" s="129">
         <v>1</v>
       </c>
-      <c r="F30" s="289">
+      <c r="F30" s="288">
         <v>20</v>
       </c>
       <c r="I30" s="129">
         <v>1</v>
       </c>
-      <c r="J30" s="289">
+      <c r="J30" s="288">
         <v>0</v>
       </c>
     </row>
@@ -28564,13 +28626,13 @@
       <c r="E31" s="129">
         <v>2</v>
       </c>
-      <c r="F31" s="289">
+      <c r="F31" s="288">
         <v>30</v>
       </c>
       <c r="I31" s="129">
         <v>2</v>
       </c>
-      <c r="J31" s="289">
+      <c r="J31" s="288">
         <v>20</v>
       </c>
     </row>
@@ -28581,13 +28643,13 @@
       <c r="E32" s="129">
         <v>3</v>
       </c>
-      <c r="F32" s="289">
+      <c r="F32" s="288">
         <v>40</v>
       </c>
       <c r="I32" s="129">
         <v>3</v>
       </c>
-      <c r="J32" s="289">
+      <c r="J32" s="288">
         <v>30</v>
       </c>
     </row>
@@ -28598,13 +28660,13 @@
       <c r="E33" s="129">
         <v>4</v>
       </c>
-      <c r="F33" s="289">
+      <c r="F33" s="288">
         <v>50</v>
       </c>
       <c r="I33" s="129">
         <v>4</v>
       </c>
-      <c r="J33" s="289">
+      <c r="J33" s="288">
         <v>40</v>
       </c>
     </row>
@@ -31250,7 +31312,7 @@
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
-      <c r="K3" s="291" t="s">
+      <c r="K3" s="290" t="s">
         <v>1114</v>
       </c>
       <c r="L3" s="31"/>
@@ -31500,7 +31562,7 @@
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
-      <c r="H22" s="291" t="s">
+      <c r="H22" s="290" t="s">
         <v>2809</v>
       </c>
       <c r="I22" s="31"/>
@@ -31520,7 +31582,7 @@
       <c r="E23" s="38"/>
       <c r="F23" s="38"/>
       <c r="G23" s="27"/>
-      <c r="H23" s="292" t="s">
+      <c r="H23" s="291" t="s">
         <v>1802</v>
       </c>
       <c r="I23" s="241" t="s">
@@ -31542,7 +31604,7 @@
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
       <c r="G24" s="27"/>
-      <c r="H24" s="292" t="s">
+      <c r="H24" s="291" t="s">
         <v>2361</v>
       </c>
       <c r="I24" s="241" t="s">
@@ -31560,7 +31622,7 @@
       <c r="E25" s="38"/>
       <c r="F25" s="38"/>
       <c r="G25" s="27"/>
-      <c r="H25" s="292" t="s">
+      <c r="H25" s="291" t="s">
         <v>2362</v>
       </c>
       <c r="I25" s="241" t="s">
@@ -31575,11 +31637,11 @@
       <c r="E26" s="38" t="s">
         <v>413</v>
       </c>
-      <c r="F26" s="295" t="s">
+      <c r="F26" s="294" t="s">
         <v>2812</v>
       </c>
       <c r="G26" s="27"/>
-      <c r="H26" s="292" t="s">
+      <c r="H26" s="291" t="s">
         <v>2377</v>
       </c>
       <c r="I26" s="240" t="s">
@@ -31594,7 +31656,7 @@
       <c r="E27" s="38"/>
       <c r="F27" s="38"/>
       <c r="G27" s="27"/>
-      <c r="H27" s="292" t="s">
+      <c r="H27" s="291" t="s">
         <v>2487</v>
       </c>
       <c r="I27" s="241" t="s">
@@ -31612,7 +31674,7 @@
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
       <c r="G28" s="27"/>
-      <c r="H28" s="292" t="s">
+      <c r="H28" s="291" t="s">
         <v>2805</v>
       </c>
       <c r="I28" s="240" t="s">
@@ -31629,7 +31691,7 @@
       <c r="D29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="27"/>
-      <c r="H29" s="292" t="s">
+      <c r="H29" s="291" t="s">
         <v>2806</v>
       </c>
       <c r="I29" s="241" t="s">
@@ -31647,7 +31709,7 @@
       <c r="E30" s="38"/>
       <c r="F30" s="38"/>
       <c r="G30" s="27"/>
-      <c r="H30" s="292" t="s">
+      <c r="H30" s="291" t="s">
         <v>2807</v>
       </c>
       <c r="I30" s="241"/>
@@ -31661,7 +31723,7 @@
       <c r="C31" s="50"/>
       <c r="F31" s="38"/>
       <c r="G31" s="27"/>
-      <c r="H31" s="292" t="s">
+      <c r="H31" s="291" t="s">
         <v>2808</v>
       </c>
       <c r="I31" s="240"/>
@@ -31674,8 +31736,8 @@
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
-      <c r="H32" s="293"/>
-      <c r="I32" s="294"/>
+      <c r="H32" s="292"/>
+      <c r="I32" s="293"/>
       <c r="J32" s="37"/>
       <c r="K32" s="34"/>
     </row>
@@ -37205,24 +37267,24 @@
     <row r="17" spans="1:14" s="108" customFormat="1"/>
     <row r="22" spans="1:14" ht="15.75" thickBot="1">
       <c r="A22" s="106"/>
-      <c r="B22" s="362" t="s">
+      <c r="B22" s="364" t="s">
         <v>1233</v>
       </c>
-      <c r="C22" s="362"/>
+      <c r="C22" s="364"/>
       <c r="D22" s="106"/>
       <c r="E22" s="106"/>
-      <c r="F22" s="362" t="s">
+      <c r="F22" s="364" t="s">
         <v>1337</v>
       </c>
-      <c r="G22" s="362"/>
-      <c r="H22" s="362"/>
+      <c r="G22" s="364"/>
+      <c r="H22" s="364"/>
       <c r="I22" s="106"/>
       <c r="J22" s="106"/>
-      <c r="K22" s="362" t="s">
+      <c r="K22" s="364" t="s">
         <v>1235</v>
       </c>
-      <c r="L22" s="362"/>
-      <c r="M22" s="362"/>
+      <c r="L22" s="364"/>
+      <c r="M22" s="364"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14">
@@ -37331,7 +37393,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="106"/>
-      <c r="B28" s="297" t="s">
+      <c r="B28" s="296" t="s">
         <v>2837</v>
       </c>
       <c r="C28" s="75"/>
@@ -37353,7 +37415,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="106"/>
-      <c r="B29" s="297" t="s">
+      <c r="B29" s="296" t="s">
         <v>2838</v>
       </c>
       <c r="C29" s="75"/>
@@ -37530,7 +37592,7 @@
       <c r="G39" s="36"/>
       <c r="H39" s="37"/>
       <c r="K39" s="35"/>
-      <c r="L39" s="294"/>
+      <c r="L39" s="293"/>
       <c r="M39" s="37"/>
       <c r="P39" t="s">
         <v>1238</v>
@@ -39649,19 +39711,19 @@
       <c r="A2" t="s">
         <v>2841</v>
       </c>
-      <c r="B2" s="290">
+      <c r="B2" s="289">
         <v>0</v>
       </c>
-      <c r="C2" s="290" t="s">
+      <c r="C2" s="289" t="s">
         <v>412</v>
       </c>
       <c r="E2" t="s">
         <v>1380</v>
       </c>
-      <c r="F2" s="290">
+      <c r="F2" s="289">
         <v>0</v>
       </c>
-      <c r="G2" s="290" t="s">
+      <c r="G2" s="289" t="s">
         <v>412</v>
       </c>
       <c r="I2" t="s">
@@ -39674,102 +39736,102 @@
       <c r="L2" t="s">
         <v>1404</v>
       </c>
-      <c r="M2" s="290" t="s">
+      <c r="M2" s="289" t="s">
         <v>412</v>
       </c>
-      <c r="N2" s="290">
+      <c r="N2" s="289">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:31">
-      <c r="B3" s="290">
+      <c r="B3" s="289">
         <v>1</v>
       </c>
-      <c r="C3" s="290" t="s">
+      <c r="C3" s="289" t="s">
         <v>524</v>
       </c>
-      <c r="F3" s="290">
+      <c r="F3" s="289">
         <v>1</v>
       </c>
-      <c r="G3" s="290" t="s">
+      <c r="G3" s="289" t="s">
         <v>524</v>
       </c>
       <c r="J3" s="43" t="s">
         <v>524</v>
       </c>
       <c r="K3" s="43"/>
-      <c r="M3" s="290" t="s">
+      <c r="M3" s="289" t="s">
         <v>524</v>
       </c>
-      <c r="N3" s="290">
+      <c r="N3" s="289">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:31">
-      <c r="B4" s="290">
+      <c r="B4" s="289">
         <v>2</v>
       </c>
-      <c r="C4" s="290" t="s">
+      <c r="C4" s="289" t="s">
         <v>559</v>
       </c>
-      <c r="F4" s="290">
+      <c r="F4" s="289">
         <v>2</v>
       </c>
-      <c r="G4" s="290" t="s">
+      <c r="G4" s="289" t="s">
         <v>559</v>
       </c>
       <c r="J4" s="43" t="s">
         <v>559</v>
       </c>
       <c r="K4" s="43"/>
-      <c r="M4" s="290" t="s">
+      <c r="M4" s="289" t="s">
         <v>559</v>
       </c>
-      <c r="N4" s="290">
+      <c r="N4" s="289">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:31">
-      <c r="B5" s="290">
+      <c r="B5" s="289">
         <v>3</v>
       </c>
-      <c r="C5" s="290" t="s">
+      <c r="C5" s="289" t="s">
         <v>412</v>
       </c>
-      <c r="F5" s="290">
+      <c r="F5" s="289">
         <v>3</v>
       </c>
-      <c r="G5" s="290" t="s">
+      <c r="G5" s="289" t="s">
         <v>412</v>
       </c>
       <c r="J5" s="43" t="s">
         <v>1689</v>
       </c>
       <c r="K5" s="43"/>
-      <c r="M5" s="290" t="s">
+      <c r="M5" s="289" t="s">
         <v>1689</v>
       </c>
-      <c r="N5" s="290">
+      <c r="N5" s="289">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:31">
-      <c r="B6" s="290">
+      <c r="B6" s="289">
         <v>4</v>
       </c>
-      <c r="C6" s="290" t="s">
+      <c r="C6" s="289" t="s">
         <v>1689</v>
       </c>
-      <c r="F6" s="290">
+      <c r="F6" s="289">
         <v>4</v>
       </c>
-      <c r="G6" s="290" t="s">
+      <c r="G6" s="289" t="s">
         <v>1689</v>
       </c>
       <c r="J6" s="43"/>
       <c r="K6" s="43"/>
-      <c r="M6" s="290"/>
-      <c r="N6" s="290"/>
+      <c r="M6" s="289"/>
+      <c r="N6" s="289"/>
     </row>
     <row r="7" spans="1:31">
       <c r="M7" s="242" t="s">
@@ -39780,56 +39842,56 @@
       </c>
     </row>
     <row r="8" spans="1:31">
-      <c r="B8" s="364" t="s">
+      <c r="B8" s="366" t="s">
         <v>2843</v>
       </c>
-      <c r="C8" s="364"/>
-      <c r="F8" s="364" t="s">
+      <c r="C8" s="366"/>
+      <c r="F8" s="366" t="s">
         <v>2844</v>
       </c>
-      <c r="G8" s="364"/>
-      <c r="I8" s="364" t="s">
+      <c r="G8" s="366"/>
+      <c r="I8" s="366" t="s">
         <v>2844</v>
       </c>
-      <c r="J8" s="364"/>
+      <c r="J8" s="366"/>
       <c r="M8" s="242" t="s">
         <v>2901</v>
       </c>
     </row>
     <row r="9" spans="1:31">
-      <c r="F9" s="364" t="s">
+      <c r="F9" s="366" t="s">
         <v>2845</v>
       </c>
-      <c r="G9" s="364"/>
-      <c r="I9" s="364" t="s">
+      <c r="G9" s="366"/>
+      <c r="I9" s="366" t="s">
         <v>2846</v>
       </c>
-      <c r="J9" s="364"/>
-      <c r="M9" s="365" t="s">
+      <c r="J9" s="366"/>
+      <c r="M9" s="367" t="s">
         <v>2844</v>
       </c>
-      <c r="N9" s="365"/>
+      <c r="N9" s="367"/>
     </row>
     <row r="10" spans="1:31">
-      <c r="M10" s="302" t="s">
+      <c r="M10" s="301" t="s">
         <v>2847</v>
       </c>
-      <c r="N10" s="302"/>
+      <c r="N10" s="301"/>
     </row>
     <row r="11" spans="1:31">
-      <c r="E11" s="363" t="s">
+      <c r="E11" s="365" t="s">
         <v>2848</v>
       </c>
-      <c r="F11" s="363"/>
-      <c r="G11" s="363"/>
-      <c r="H11" s="363"/>
-      <c r="I11" s="363"/>
-      <c r="J11" s="363"/>
-      <c r="K11" s="363"/>
-      <c r="L11" s="363"/>
-      <c r="M11" s="363"/>
-      <c r="N11" s="363"/>
-      <c r="O11" s="363"/>
+      <c r="F11" s="365"/>
+      <c r="G11" s="365"/>
+      <c r="H11" s="365"/>
+      <c r="I11" s="365"/>
+      <c r="J11" s="365"/>
+      <c r="K11" s="365"/>
+      <c r="L11" s="365"/>
+      <c r="M11" s="365"/>
+      <c r="N11" s="365"/>
+      <c r="O11" s="365"/>
     </row>
     <row r="12" spans="1:31">
       <c r="A12" t="s">
@@ -39870,7 +39932,7 @@
       <c r="J14" s="43" t="s">
         <v>412</v>
       </c>
-      <c r="L14" s="299" t="s">
+      <c r="L14" s="298" t="s">
         <v>412</v>
       </c>
       <c r="M14" s="43" t="s">
@@ -39892,7 +39954,7 @@
       <c r="J15" s="43" t="s">
         <v>524</v>
       </c>
-      <c r="L15" s="299" t="s">
+      <c r="L15" s="298" t="s">
         <v>524</v>
       </c>
       <c r="M15" s="43" t="s">
@@ -39912,7 +39974,7 @@
       <c r="J16" s="43" t="s">
         <v>559</v>
       </c>
-      <c r="L16" s="299" t="s">
+      <c r="L16" s="298" t="s">
         <v>559</v>
       </c>
       <c r="M16" s="43" t="s">
@@ -40008,7 +40070,7 @@
       <c r="AE19" s="27"/>
     </row>
     <row r="20" spans="1:32">
-      <c r="C20" s="298" t="s">
+      <c r="C20" s="297" t="s">
         <v>412</v>
       </c>
       <c r="D20" s="43" t="s">
@@ -40047,7 +40109,7 @@
       <c r="AE20" s="27"/>
     </row>
     <row r="21" spans="1:32">
-      <c r="C21" s="298" t="s">
+      <c r="C21" s="297" t="s">
         <v>524</v>
       </c>
       <c r="D21" s="43" t="s">
@@ -40083,7 +40145,7 @@
       <c r="AE21" s="27"/>
     </row>
     <row r="22" spans="1:32">
-      <c r="C22" s="298" t="s">
+      <c r="C22" s="297" t="s">
         <v>559</v>
       </c>
       <c r="D22" s="43" t="s">
@@ -40352,16 +40414,16 @@
       <c r="AE31" s="27"/>
     </row>
     <row r="32" spans="1:32">
-      <c r="E32" s="300" t="s">
+      <c r="E32" s="299" t="s">
         <v>2862</v>
       </c>
       <c r="G32" s="43" t="s">
         <v>2864</v>
       </c>
-      <c r="I32" s="300" t="s">
+      <c r="I32" s="299" t="s">
         <v>2862</v>
       </c>
-      <c r="K32" s="300"/>
+      <c r="K32" s="299"/>
       <c r="M32" s="27"/>
       <c r="N32" s="27"/>
       <c r="O32" s="27"/>
@@ -40386,12 +40448,12 @@
       </c>
     </row>
     <row r="33" spans="1:32">
-      <c r="E33" s="300"/>
+      <c r="E33" s="299"/>
       <c r="G33" s="43" t="s">
         <v>2865</v>
       </c>
-      <c r="I33" s="300"/>
-      <c r="K33" s="300"/>
+      <c r="I33" s="299"/>
+      <c r="K33" s="299"/>
       <c r="M33" s="27"/>
       <c r="N33" s="27"/>
       <c r="O33" s="27"/>
@@ -40416,12 +40478,12 @@
       </c>
     </row>
     <row r="34" spans="1:32">
-      <c r="E34" s="300"/>
+      <c r="E34" s="299"/>
       <c r="G34" s="43" t="s">
         <v>2866</v>
       </c>
-      <c r="I34" s="300"/>
-      <c r="K34" s="300"/>
+      <c r="I34" s="299"/>
+      <c r="K34" s="299"/>
       <c r="M34" s="27"/>
       <c r="N34" s="27"/>
       <c r="O34" s="27"/>
@@ -41109,10 +41171,10 @@
       </c>
     </row>
     <row r="78" spans="1:18">
-      <c r="B78" s="296" t="s">
+      <c r="B78" s="295" t="s">
         <v>412</v>
       </c>
-      <c r="C78" s="296">
+      <c r="C78" s="295">
         <v>50</v>
       </c>
       <c r="F78" t="s">
@@ -41120,10 +41182,10 @@
       </c>
     </row>
     <row r="79" spans="1:18">
-      <c r="B79" s="296" t="s">
+      <c r="B79" s="295" t="s">
         <v>524</v>
       </c>
-      <c r="C79" s="296">
+      <c r="C79" s="295">
         <v>80</v>
       </c>
       <c r="F79" t="s">
@@ -41131,10 +41193,10 @@
       </c>
     </row>
     <row r="80" spans="1:18">
-      <c r="B80" s="296" t="s">
+      <c r="B80" s="295" t="s">
         <v>559</v>
       </c>
-      <c r="C80" s="296">
+      <c r="C80" s="295">
         <v>20</v>
       </c>
       <c r="L80" t="s">
@@ -41142,10 +41204,10 @@
       </c>
     </row>
     <row r="81" spans="2:12">
-      <c r="B81" s="296" t="s">
+      <c r="B81" s="295" t="s">
         <v>1689</v>
       </c>
-      <c r="C81" s="296">
+      <c r="C81" s="295">
         <v>80</v>
       </c>
       <c r="E81" s="125" t="s">
@@ -41157,17 +41219,17 @@
       <c r="K81" t="s">
         <v>48</v>
       </c>
-      <c r="L81" s="296" t="s">
+      <c r="L81" s="295" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="82" spans="2:12">
-      <c r="B82" s="296"/>
-      <c r="C82" s="296"/>
+      <c r="B82" s="295"/>
+      <c r="C82" s="295"/>
       <c r="F82" t="s">
         <v>2906</v>
       </c>
-      <c r="L82" s="296" t="s">
+      <c r="L82" s="295" t="s">
         <v>524</v>
       </c>
     </row>
@@ -41175,7 +41237,7 @@
       <c r="F83" t="s">
         <v>366</v>
       </c>
-      <c r="L83" s="296" t="s">
+      <c r="L83" s="295" t="s">
         <v>559</v>
       </c>
     </row>
@@ -41183,7 +41245,7 @@
       <c r="G84" t="s">
         <v>2907</v>
       </c>
-      <c r="L84" s="296" t="s">
+      <c r="L84" s="295" t="s">
         <v>1689</v>
       </c>
     </row>
@@ -43160,7 +43222,7 @@
       <c r="H2" s="248"/>
       <c r="I2" s="248"/>
       <c r="J2" s="248"/>
-      <c r="K2" s="301" t="s">
+      <c r="K2" s="300" t="s">
         <v>413</v>
       </c>
       <c r="L2" s="121" t="s">
@@ -43589,11 +43651,11 @@
       <c r="L6" s="43" t="s">
         <v>1509</v>
       </c>
-      <c r="M6" s="366" t="s">
+      <c r="M6" s="368" t="s">
         <v>1510</v>
       </c>
-      <c r="N6" s="366"/>
-      <c r="O6" s="366"/>
+      <c r="N6" s="368"/>
+      <c r="O6" s="368"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
@@ -44766,10 +44828,10 @@
       </c>
       <c r="G121" s="30"/>
       <c r="H121" s="31"/>
-      <c r="I121" s="345" t="s">
+      <c r="I121" s="347" t="s">
         <v>3018</v>
       </c>
-      <c r="J121" s="345" t="s">
+      <c r="J121" s="347" t="s">
         <v>3022</v>
       </c>
       <c r="K121" s="27"/>
@@ -44785,8 +44847,8 @@
       <c r="H122" s="27" t="s">
         <v>559</v>
       </c>
-      <c r="I122" s="346"/>
-      <c r="J122" s="346"/>
+      <c r="I122" s="348"/>
+      <c r="J122" s="348"/>
       <c r="K122" s="27"/>
       <c r="L122" s="27"/>
       <c r="M122" s="34"/>
@@ -44800,8 +44862,8 @@
       <c r="H123" s="27">
         <v>19</v>
       </c>
-      <c r="I123" s="346"/>
-      <c r="J123" s="346"/>
+      <c r="I123" s="348"/>
+      <c r="J123" s="348"/>
       <c r="K123" s="27"/>
       <c r="L123" s="27"/>
       <c r="M123" s="34"/>
@@ -44815,8 +44877,8 @@
       <c r="H124" s="36" t="s">
         <v>2036</v>
       </c>
-      <c r="I124" s="346"/>
-      <c r="J124" s="346"/>
+      <c r="I124" s="348"/>
+      <c r="J124" s="348"/>
       <c r="K124" s="27"/>
       <c r="L124" s="27"/>
       <c r="M124" s="34"/>
@@ -44826,8 +44888,8 @@
       <c r="F125" s="27"/>
       <c r="G125" s="27"/>
       <c r="H125" s="27"/>
-      <c r="I125" s="346"/>
-      <c r="J125" s="346"/>
+      <c r="I125" s="348"/>
+      <c r="J125" s="348"/>
       <c r="K125" s="27"/>
       <c r="L125" s="27"/>
       <c r="M125" s="34"/>
@@ -44840,8 +44902,8 @@
       <c r="F126" s="27"/>
       <c r="G126" s="27"/>
       <c r="H126" s="27"/>
-      <c r="I126" s="346"/>
-      <c r="J126" s="346"/>
+      <c r="I126" s="348"/>
+      <c r="J126" s="348"/>
       <c r="K126" s="27"/>
       <c r="L126" s="27"/>
       <c r="M126" s="34"/>
@@ -44853,8 +44915,8 @@
       </c>
       <c r="G127" s="30"/>
       <c r="H127" s="31"/>
-      <c r="I127" s="346"/>
-      <c r="J127" s="346"/>
+      <c r="I127" s="348"/>
+      <c r="J127" s="348"/>
       <c r="K127" s="27"/>
       <c r="L127" s="27"/>
       <c r="M127" s="34"/>
@@ -44868,8 +44930,8 @@
       <c r="H128" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="I128" s="346"/>
-      <c r="J128" s="346"/>
+      <c r="I128" s="348"/>
+      <c r="J128" s="348"/>
       <c r="K128" s="27"/>
       <c r="L128" s="27"/>
       <c r="M128" s="34"/>
@@ -44883,8 +44945,8 @@
       <c r="H129" s="27">
         <v>20</v>
       </c>
-      <c r="I129" s="346"/>
-      <c r="J129" s="346"/>
+      <c r="I129" s="348"/>
+      <c r="J129" s="348"/>
       <c r="K129" s="27"/>
       <c r="L129" s="27"/>
       <c r="M129" s="34"/>
@@ -44898,8 +44960,8 @@
       <c r="H130" s="36" t="s">
         <v>3014</v>
       </c>
-      <c r="I130" s="346"/>
-      <c r="J130" s="346"/>
+      <c r="I130" s="348"/>
+      <c r="J130" s="348"/>
       <c r="K130" s="27"/>
       <c r="L130" s="27"/>
       <c r="M130" s="34"/>
@@ -44909,8 +44971,8 @@
       <c r="F131" s="27"/>
       <c r="G131" s="27"/>
       <c r="H131" s="27"/>
-      <c r="I131" s="346"/>
-      <c r="J131" s="346"/>
+      <c r="I131" s="348"/>
+      <c r="J131" s="348"/>
       <c r="K131" s="27"/>
       <c r="L131" s="27"/>
       <c r="M131" s="34"/>
@@ -44922,8 +44984,8 @@
       </c>
       <c r="G132" s="30"/>
       <c r="H132" s="31"/>
-      <c r="I132" s="346"/>
-      <c r="J132" s="346"/>
+      <c r="I132" s="348"/>
+      <c r="J132" s="348"/>
       <c r="K132" s="27"/>
       <c r="L132" s="27"/>
       <c r="M132" s="34"/>
@@ -44937,8 +44999,8 @@
       <c r="H133" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="I133" s="346"/>
-      <c r="J133" s="346"/>
+      <c r="I133" s="348"/>
+      <c r="J133" s="348"/>
       <c r="K133" s="27"/>
       <c r="L133" s="27"/>
       <c r="M133" s="34"/>
@@ -44952,8 +45014,8 @@
       <c r="H134" s="27">
         <v>18</v>
       </c>
-      <c r="I134" s="346"/>
-      <c r="J134" s="346"/>
+      <c r="I134" s="348"/>
+      <c r="J134" s="348"/>
       <c r="K134" s="27"/>
       <c r="L134" s="27"/>
       <c r="M134" s="34"/>
@@ -44967,8 +45029,8 @@
       <c r="H135" s="36" t="s">
         <v>3015</v>
       </c>
-      <c r="I135" s="347"/>
-      <c r="J135" s="347"/>
+      <c r="I135" s="349"/>
+      <c r="J135" s="349"/>
       <c r="K135" s="27"/>
       <c r="L135" s="27"/>
       <c r="M135" s="34"/>
@@ -45048,8 +45110,8 @@
       <c r="H147" s="31" t="s">
         <v>3021</v>
       </c>
-      <c r="I147" s="348"/>
-      <c r="J147" s="348"/>
+      <c r="I147" s="350"/>
+      <c r="J147" s="350"/>
       <c r="K147" s="27"/>
       <c r="L147" s="27"/>
       <c r="M147" s="34"/>
@@ -45063,8 +45125,8 @@
       <c r="H148" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="I148" s="349"/>
-      <c r="J148" s="349"/>
+      <c r="I148" s="351"/>
+      <c r="J148" s="351"/>
       <c r="K148" s="27"/>
       <c r="L148" s="27"/>
       <c r="M148" s="34"/>
@@ -45078,8 +45140,8 @@
       <c r="H149" s="27">
         <v>19</v>
       </c>
-      <c r="I149" s="349"/>
-      <c r="J149" s="349"/>
+      <c r="I149" s="351"/>
+      <c r="J149" s="351"/>
       <c r="K149" s="27"/>
       <c r="L149" s="27"/>
       <c r="M149" s="34"/>
@@ -45093,8 +45155,8 @@
       <c r="H150" s="36" t="s">
         <v>2036</v>
       </c>
-      <c r="I150" s="349"/>
-      <c r="J150" s="349"/>
+      <c r="I150" s="351"/>
+      <c r="J150" s="351"/>
       <c r="K150" s="27"/>
       <c r="L150" s="27"/>
       <c r="M150" s="34"/>
@@ -45104,8 +45166,8 @@
       <c r="F151" s="27"/>
       <c r="G151" s="27"/>
       <c r="H151" s="27"/>
-      <c r="I151" s="349"/>
-      <c r="J151" s="349"/>
+      <c r="I151" s="351"/>
+      <c r="J151" s="351"/>
       <c r="K151" s="27"/>
       <c r="L151" s="27"/>
       <c r="M151" s="34"/>
@@ -45115,8 +45177,8 @@
       <c r="F152" s="27"/>
       <c r="G152" s="27"/>
       <c r="H152" s="27"/>
-      <c r="I152" s="349"/>
-      <c r="J152" s="349"/>
+      <c r="I152" s="351"/>
+      <c r="J152" s="351"/>
       <c r="K152" s="27"/>
       <c r="L152" s="27"/>
       <c r="M152" s="34"/>
@@ -45132,8 +45194,8 @@
       <c r="H153" s="31" t="s">
         <v>3021</v>
       </c>
-      <c r="I153" s="349"/>
-      <c r="J153" s="349"/>
+      <c r="I153" s="351"/>
+      <c r="J153" s="351"/>
       <c r="K153" s="27"/>
       <c r="L153" s="27"/>
       <c r="M153" s="34"/>
@@ -45150,8 +45212,8 @@
       <c r="H154" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="I154" s="349"/>
-      <c r="J154" s="349"/>
+      <c r="I154" s="351"/>
+      <c r="J154" s="351"/>
       <c r="K154" s="27"/>
       <c r="L154" s="27"/>
       <c r="M154" s="34"/>
@@ -45165,8 +45227,8 @@
       <c r="H155" s="27">
         <v>20</v>
       </c>
-      <c r="I155" s="349"/>
-      <c r="J155" s="349"/>
+      <c r="I155" s="351"/>
+      <c r="J155" s="351"/>
       <c r="K155" s="27"/>
       <c r="L155" s="27"/>
       <c r="M155" s="34"/>
@@ -45180,8 +45242,8 @@
       <c r="H156" s="36" t="s">
         <v>3014</v>
       </c>
-      <c r="I156" s="349"/>
-      <c r="J156" s="349"/>
+      <c r="I156" s="351"/>
+      <c r="J156" s="351"/>
       <c r="K156" s="27"/>
       <c r="L156" s="27"/>
       <c r="M156" s="34"/>
@@ -45191,8 +45253,8 @@
       <c r="F157" s="27"/>
       <c r="G157" s="27"/>
       <c r="H157" s="27"/>
-      <c r="I157" s="349"/>
-      <c r="J157" s="349"/>
+      <c r="I157" s="351"/>
+      <c r="J157" s="351"/>
       <c r="K157" s="27"/>
       <c r="L157" s="27"/>
       <c r="M157" s="34"/>
@@ -45208,8 +45270,8 @@
       <c r="H158" s="31" t="s">
         <v>3021</v>
       </c>
-      <c r="I158" s="349"/>
-      <c r="J158" s="349"/>
+      <c r="I158" s="351"/>
+      <c r="J158" s="351"/>
       <c r="K158" s="27"/>
       <c r="L158" s="27"/>
       <c r="M158" s="34"/>
@@ -45223,8 +45285,8 @@
       <c r="H159" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="I159" s="349"/>
-      <c r="J159" s="349"/>
+      <c r="I159" s="351"/>
+      <c r="J159" s="351"/>
       <c r="K159" s="27"/>
       <c r="L159" s="27"/>
       <c r="M159" s="34"/>
@@ -45238,8 +45300,8 @@
       <c r="H160" s="27">
         <v>18</v>
       </c>
-      <c r="I160" s="349"/>
-      <c r="J160" s="349"/>
+      <c r="I160" s="351"/>
+      <c r="J160" s="351"/>
       <c r="K160" s="27"/>
       <c r="L160" s="27"/>
       <c r="M160" s="34"/>
@@ -45253,8 +45315,8 @@
       <c r="H161" s="36" t="s">
         <v>3015</v>
       </c>
-      <c r="I161" s="350"/>
-      <c r="J161" s="350"/>
+      <c r="I161" s="352"/>
+      <c r="J161" s="352"/>
       <c r="K161" s="27"/>
       <c r="L161" s="27"/>
       <c r="M161" s="34"/>
@@ -46213,7 +46275,7 @@
       <c r="F269" s="39">
         <v>9</v>
       </c>
-      <c r="G269" s="343" t="s">
+      <c r="G269" s="345" t="s">
         <v>2589</v>
       </c>
       <c r="I269" s="56" t="s">
@@ -46234,7 +46296,7 @@
       <c r="F270" s="39">
         <v>15</v>
       </c>
-      <c r="G270" s="344"/>
+      <c r="G270" s="346"/>
       <c r="I270" s="167" t="s">
         <v>2585</v>
       </c>
@@ -48181,17 +48243,17 @@
       <c r="A2" t="s">
         <v>3049</v>
       </c>
-      <c r="E2" s="341" t="s">
+      <c r="E2" s="343" t="s">
         <v>3057</v>
       </c>
-      <c r="F2" s="351"/>
-      <c r="G2" s="351"/>
-      <c r="H2" s="351"/>
-      <c r="I2" s="351"/>
-      <c r="J2" s="351"/>
-      <c r="K2" s="351"/>
-      <c r="L2" s="351"/>
-      <c r="M2" s="342"/>
+      <c r="F2" s="353"/>
+      <c r="G2" s="353"/>
+      <c r="H2" s="353"/>
+      <c r="I2" s="353"/>
+      <c r="J2" s="353"/>
+      <c r="K2" s="353"/>
+      <c r="L2" s="353"/>
+      <c r="M2" s="344"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1">
       <c r="B3" t="s">
@@ -48200,10 +48262,10 @@
       <c r="C3" t="s">
         <v>2584</v>
       </c>
-      <c r="E3" s="311" t="s">
+      <c r="E3" s="310" t="s">
         <v>1593</v>
       </c>
-      <c r="F3" s="312" t="s">
+      <c r="F3" s="311" t="s">
         <v>2184</v>
       </c>
       <c r="G3" s="27"/>
@@ -48477,17 +48539,17 @@
       <c r="A23" t="s">
         <v>3049</v>
       </c>
-      <c r="E23" s="341" t="s">
+      <c r="E23" s="343" t="s">
         <v>3057</v>
       </c>
-      <c r="F23" s="351"/>
-      <c r="G23" s="351"/>
-      <c r="H23" s="351"/>
-      <c r="I23" s="351"/>
-      <c r="J23" s="351"/>
-      <c r="K23" s="351"/>
-      <c r="L23" s="351"/>
-      <c r="M23" s="342"/>
+      <c r="F23" s="353"/>
+      <c r="G23" s="353"/>
+      <c r="H23" s="353"/>
+      <c r="I23" s="353"/>
+      <c r="J23" s="353"/>
+      <c r="K23" s="353"/>
+      <c r="L23" s="353"/>
+      <c r="M23" s="344"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1">
       <c r="B24" t="s">
@@ -48496,10 +48558,10 @@
       <c r="C24" t="s">
         <v>2584</v>
       </c>
-      <c r="E24" s="311" t="s">
+      <c r="E24" s="310" t="s">
         <v>1593</v>
       </c>
-      <c r="F24" s="312" t="s">
+      <c r="F24" s="311" t="s">
         <v>2184</v>
       </c>
       <c r="G24" s="27"/>
@@ -48763,17 +48825,17 @@
       <c r="A42" t="s">
         <v>3049</v>
       </c>
-      <c r="E42" s="341" t="s">
+      <c r="E42" s="343" t="s">
         <v>3057</v>
       </c>
-      <c r="F42" s="351"/>
-      <c r="G42" s="351"/>
-      <c r="H42" s="351"/>
-      <c r="I42" s="351"/>
-      <c r="J42" s="351"/>
-      <c r="K42" s="351"/>
-      <c r="L42" s="351"/>
-      <c r="M42" s="342"/>
+      <c r="F42" s="353"/>
+      <c r="G42" s="353"/>
+      <c r="H42" s="353"/>
+      <c r="I42" s="353"/>
+      <c r="J42" s="353"/>
+      <c r="K42" s="353"/>
+      <c r="L42" s="353"/>
+      <c r="M42" s="344"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1">
       <c r="B43" t="s">
@@ -48782,10 +48844,10 @@
       <c r="C43" t="s">
         <v>2584</v>
       </c>
-      <c r="E43" s="311" t="s">
+      <c r="E43" s="310" t="s">
         <v>1593</v>
       </c>
-      <c r="F43" s="312" t="s">
+      <c r="F43" s="311" t="s">
         <v>2184</v>
       </c>
       <c r="G43" s="27"/>
@@ -49069,32 +49131,32 @@
     </row>
     <row r="63" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="64" spans="1:15" ht="23.25">
-      <c r="A64" s="325" t="s">
+      <c r="A64" s="324" t="s">
         <v>3088</v>
       </c>
-      <c r="B64" s="325"/>
-      <c r="C64" s="325"/>
-      <c r="D64" s="325"/>
-      <c r="G64" s="341" t="s">
+      <c r="B64" s="324"/>
+      <c r="C64" s="324"/>
+      <c r="D64" s="324"/>
+      <c r="G64" s="343" t="s">
         <v>3057</v>
       </c>
-      <c r="H64" s="351"/>
-      <c r="I64" s="351"/>
-      <c r="J64" s="351"/>
-      <c r="K64" s="351"/>
-      <c r="L64" s="351"/>
-      <c r="M64" s="351"/>
-      <c r="N64" s="351"/>
-      <c r="O64" s="342"/>
+      <c r="H64" s="353"/>
+      <c r="I64" s="353"/>
+      <c r="J64" s="353"/>
+      <c r="K64" s="353"/>
+      <c r="L64" s="353"/>
+      <c r="M64" s="353"/>
+      <c r="N64" s="353"/>
+      <c r="O64" s="344"/>
     </row>
     <row r="65" spans="1:15" ht="15.75" thickBot="1">
       <c r="B65" t="s">
         <v>1635</v>
       </c>
-      <c r="G65" s="311" t="s">
+      <c r="G65" s="310" t="s">
         <v>1593</v>
       </c>
-      <c r="H65" s="324" t="s">
+      <c r="H65" s="323" t="s">
         <v>2184</v>
       </c>
       <c r="I65" s="27"/>
@@ -49116,22 +49178,22 @@
         <v>1802</v>
       </c>
       <c r="I66" s="117"/>
-      <c r="J66" s="313" t="s">
+      <c r="J66" s="312" t="s">
         <v>1802</v>
       </c>
-      <c r="K66" s="314"/>
-      <c r="L66" s="315"/>
-      <c r="M66" s="313"/>
+      <c r="K66" s="313"/>
+      <c r="L66" s="314"/>
+      <c r="M66" s="312"/>
       <c r="N66" s="51"/>
       <c r="O66" s="52"/>
     </row>
     <row r="67" spans="1:15">
-      <c r="A67" s="327"/>
-      <c r="B67" s="327" t="s">
+      <c r="A67" s="326"/>
+      <c r="B67" s="326" t="s">
         <v>3089</v>
       </c>
-      <c r="C67" s="327"/>
-      <c r="D67" s="327" t="s">
+      <c r="C67" s="326"/>
+      <c r="D67" s="326" t="s">
         <v>3100</v>
       </c>
       <c r="G67" s="50" t="s">
@@ -49141,24 +49203,24 @@
         <v>20</v>
       </c>
       <c r="I67" s="117"/>
-      <c r="J67" s="313"/>
+      <c r="J67" s="312"/>
       <c r="K67" s="50" t="s">
         <v>58</v>
       </c>
       <c r="L67" s="52" t="s">
         <v>1832</v>
       </c>
-      <c r="M67" s="321"/>
+      <c r="M67" s="320"/>
       <c r="N67" s="51"/>
       <c r="O67" s="52"/>
     </row>
     <row r="68" spans="1:15">
-      <c r="A68" s="327" t="s">
+      <c r="A68" s="326" t="s">
         <v>144</v>
       </c>
-      <c r="B68" s="327"/>
-      <c r="C68" s="327"/>
-      <c r="D68" s="327"/>
+      <c r="B68" s="326"/>
+      <c r="C68" s="326"/>
+      <c r="D68" s="326"/>
       <c r="G68" s="50" t="s">
         <v>1735</v>
       </c>
@@ -49166,24 +49228,24 @@
         <v>1802</v>
       </c>
       <c r="I68" s="51"/>
-      <c r="J68" s="313"/>
+      <c r="J68" s="312"/>
       <c r="K68" s="50" t="s">
         <v>201</v>
       </c>
-      <c r="L68" s="316">
+      <c r="L68" s="315">
         <v>0</v>
       </c>
-      <c r="M68" s="321"/>
+      <c r="M68" s="320"/>
       <c r="N68" s="51"/>
       <c r="O68" s="52"/>
     </row>
     <row r="69" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A69" s="327" t="s">
+      <c r="A69" s="326" t="s">
         <v>3090</v>
       </c>
-      <c r="B69" s="327"/>
-      <c r="C69" s="327"/>
-      <c r="D69" s="327"/>
+      <c r="B69" s="326"/>
+      <c r="C69" s="326"/>
+      <c r="D69" s="326"/>
       <c r="E69" t="s">
         <v>2398</v>
       </c>
@@ -49194,10 +49256,10 @@
         <v>20</v>
       </c>
       <c r="I69" s="51"/>
-      <c r="J69" s="313"/>
-      <c r="K69" s="317"/>
-      <c r="L69" s="322"/>
-      <c r="M69" s="323"/>
+      <c r="J69" s="312"/>
+      <c r="K69" s="316"/>
+      <c r="L69" s="321"/>
+      <c r="M69" s="322"/>
       <c r="N69" s="27"/>
       <c r="O69" s="52"/>
     </row>
@@ -49212,10 +49274,10 @@
         <v>2361</v>
       </c>
       <c r="I70" s="51"/>
-      <c r="J70" s="313"/>
-      <c r="K70" s="313"/>
-      <c r="L70" s="313"/>
-      <c r="M70" s="313"/>
+      <c r="J70" s="312"/>
+      <c r="K70" s="312"/>
+      <c r="L70" s="312"/>
+      <c r="M70" s="312"/>
       <c r="N70" s="51"/>
       <c r="O70" s="52"/>
     </row>
@@ -49233,9 +49295,9 @@
       <c r="J71" s="51" t="s">
         <v>2361</v>
       </c>
-      <c r="K71" s="314"/>
-      <c r="L71" s="315"/>
-      <c r="M71" s="313"/>
+      <c r="K71" s="313"/>
+      <c r="L71" s="314"/>
+      <c r="M71" s="312"/>
       <c r="N71" s="51"/>
       <c r="O71" s="52"/>
     </row>
@@ -49250,14 +49312,14 @@
         <v>2361</v>
       </c>
       <c r="I72" s="51"/>
-      <c r="J72" s="313"/>
+      <c r="J72" s="312"/>
       <c r="K72" s="50" t="s">
         <v>58</v>
       </c>
       <c r="L72" s="52" t="s">
         <v>1832</v>
       </c>
-      <c r="M72" s="313"/>
+      <c r="M72" s="312"/>
       <c r="N72" s="51"/>
       <c r="O72" s="52"/>
     </row>
@@ -49276,14 +49338,14 @@
         <v>30</v>
       </c>
       <c r="I73" s="51"/>
-      <c r="J73" s="313"/>
+      <c r="J73" s="312"/>
       <c r="K73" s="50" t="s">
         <v>201</v>
       </c>
-      <c r="L73" s="316">
+      <c r="L73" s="315">
         <v>0</v>
       </c>
-      <c r="M73" s="313"/>
+      <c r="M73" s="312"/>
       <c r="N73" s="51"/>
       <c r="O73" s="52"/>
     </row>
@@ -49295,8 +49357,8 @@
       <c r="H74" s="51"/>
       <c r="I74" s="51"/>
       <c r="J74" s="51"/>
-      <c r="K74" s="317"/>
-      <c r="L74" s="322"/>
+      <c r="K74" s="316"/>
+      <c r="L74" s="321"/>
       <c r="M74" s="51"/>
       <c r="N74" s="51"/>
       <c r="O74" s="52"/>
@@ -49415,10 +49477,10 @@
       </c>
     </row>
     <row r="82" spans="1:15" ht="28.5">
-      <c r="A82" s="326" t="s">
+      <c r="A82" s="325" t="s">
         <v>3095</v>
       </c>
-      <c r="B82" s="326"/>
+      <c r="B82" s="325"/>
       <c r="D82" t="s">
         <v>3107</v>
       </c>
@@ -49595,7 +49657,7 @@
       <c r="J93" s="27"/>
       <c r="K93" s="34"/>
       <c r="L93" s="27"/>
-      <c r="M93" s="318"/>
+      <c r="M93" s="317"/>
       <c r="N93" s="27"/>
       <c r="O93" s="27"/>
     </row>
@@ -49646,7 +49708,7 @@
       <c r="F96" s="27"/>
       <c r="G96" s="27"/>
       <c r="H96" s="27"/>
-      <c r="I96" s="318"/>
+      <c r="I96" s="317"/>
       <c r="J96" s="27"/>
       <c r="K96" s="27"/>
       <c r="L96" s="27"/>
@@ -51032,8 +51094,8 @@
       <c r="O177" s="27"/>
     </row>
     <row r="178" spans="1:15">
-      <c r="A178" s="319"/>
-      <c r="B178" s="319"/>
+      <c r="A178" s="318"/>
+      <c r="B178" s="318"/>
       <c r="C178" s="172"/>
       <c r="D178" s="27"/>
       <c r="E178" s="27"/>
@@ -51049,8 +51111,8 @@
       <c r="O178" s="27"/>
     </row>
     <row r="179" spans="1:15">
-      <c r="A179" s="319"/>
-      <c r="B179" s="319"/>
+      <c r="A179" s="318"/>
+      <c r="B179" s="318"/>
       <c r="C179" s="27"/>
       <c r="D179" s="27"/>
       <c r="E179" s="27"/>
@@ -51424,7 +51486,7 @@
     </row>
     <row r="201" spans="1:15">
       <c r="A201" s="172"/>
-      <c r="B201" s="320"/>
+      <c r="B201" s="319"/>
       <c r="C201" s="27"/>
       <c r="D201" s="27"/>
       <c r="E201" s="51"/>
@@ -51440,7 +51502,7 @@
       <c r="O201" s="27"/>
     </row>
     <row r="202" spans="1:15">
-      <c r="A202" s="320"/>
+      <c r="A202" s="319"/>
       <c r="B202" s="27"/>
       <c r="C202" s="27"/>
       <c r="D202" s="27"/>
@@ -51849,7 +51911,7 @@
     </row>
     <row r="226" spans="1:15">
       <c r="A226" s="172"/>
-      <c r="B226" s="320"/>
+      <c r="B226" s="319"/>
       <c r="C226" s="27"/>
       <c r="D226" s="27"/>
       <c r="E226" s="51"/>
@@ -51882,7 +51944,7 @@
       <c r="O227" s="27"/>
     </row>
     <row r="228" spans="1:15">
-      <c r="A228" s="320"/>
+      <c r="A228" s="319"/>
       <c r="B228" s="27"/>
       <c r="C228" s="27"/>
       <c r="D228" s="27"/>
@@ -52030,49 +52092,49 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:13">
-      <c r="B2" s="352" t="s">
+      <c r="B2" s="354" t="s">
         <v>2405</v>
       </c>
-      <c r="C2" s="353"/>
-      <c r="D2" s="354"/>
-      <c r="F2" s="352" t="s">
+      <c r="C2" s="355"/>
+      <c r="D2" s="356"/>
+      <c r="F2" s="354" t="s">
         <v>3024</v>
       </c>
-      <c r="G2" s="353"/>
-      <c r="H2" s="353"/>
-      <c r="I2" s="354"/>
-      <c r="K2" s="352" t="s">
+      <c r="G2" s="355"/>
+      <c r="H2" s="355"/>
+      <c r="I2" s="356"/>
+      <c r="K2" s="354" t="s">
         <v>3026</v>
       </c>
-      <c r="L2" s="353"/>
-      <c r="M2" s="354"/>
+      <c r="L2" s="355"/>
+      <c r="M2" s="356"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="355"/>
-      <c r="C3" s="356"/>
-      <c r="D3" s="357"/>
-      <c r="F3" s="355"/>
-      <c r="G3" s="356"/>
-      <c r="H3" s="356"/>
-      <c r="I3" s="357"/>
-      <c r="K3" s="355"/>
-      <c r="L3" s="356"/>
-      <c r="M3" s="357"/>
+      <c r="B3" s="357"/>
+      <c r="C3" s="358"/>
+      <c r="D3" s="359"/>
+      <c r="F3" s="357"/>
+      <c r="G3" s="358"/>
+      <c r="H3" s="358"/>
+      <c r="I3" s="359"/>
+      <c r="K3" s="357"/>
+      <c r="L3" s="358"/>
+      <c r="M3" s="359"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="355"/>
-      <c r="C4" s="356"/>
-      <c r="D4" s="357"/>
-      <c r="F4" s="355"/>
-      <c r="G4" s="356"/>
-      <c r="H4" s="356"/>
-      <c r="I4" s="357"/>
-      <c r="K4" s="355"/>
-      <c r="L4" s="356"/>
-      <c r="M4" s="357"/>
+      <c r="B4" s="357"/>
+      <c r="C4" s="358"/>
+      <c r="D4" s="359"/>
+      <c r="F4" s="357"/>
+      <c r="G4" s="358"/>
+      <c r="H4" s="358"/>
+      <c r="I4" s="359"/>
+      <c r="K4" s="357"/>
+      <c r="L4" s="358"/>
+      <c r="M4" s="359"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="358" t="s">
+      <c r="A5" s="360" t="s">
         <v>2190</v>
       </c>
       <c r="B5" s="80"/>
@@ -52099,7 +52161,7 @@
       <c r="M5" s="41"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="358"/>
+      <c r="A6" s="360"/>
       <c r="B6" s="80"/>
       <c r="C6" s="39" t="s">
         <v>58</v>
@@ -52124,7 +52186,7 @@
       <c r="M6" s="41"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="358"/>
+      <c r="A7" s="360"/>
       <c r="B7" s="80"/>
       <c r="C7" s="39" t="s">
         <v>3028</v>
@@ -52157,54 +52219,54 @@
       <c r="M8" s="34"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="358" t="s">
+      <c r="A9" s="360" t="s">
         <v>203</v>
       </c>
-      <c r="B9" s="306" t="s">
+      <c r="B9" s="305" t="s">
         <v>3023</v>
       </c>
       <c r="C9" s="143"/>
       <c r="D9" s="251"/>
-      <c r="F9" s="306" t="s">
+      <c r="F9" s="305" t="s">
         <v>3031</v>
       </c>
       <c r="G9" s="143"/>
       <c r="H9" s="143"/>
       <c r="I9" s="251"/>
-      <c r="K9" s="306" t="s">
+      <c r="K9" s="305" t="s">
         <v>3030</v>
       </c>
       <c r="L9" s="143"/>
       <c r="M9" s="251"/>
     </row>
     <row r="10" spans="1:13" ht="30.75" customHeight="1">
-      <c r="A10" s="358"/>
-      <c r="B10" s="306"/>
-      <c r="C10" s="307" t="s">
+      <c r="A10" s="360"/>
+      <c r="B10" s="305"/>
+      <c r="C10" s="306" t="s">
         <v>3033</v>
       </c>
       <c r="D10" s="251"/>
       <c r="E10" t="s">
         <v>3035</v>
       </c>
-      <c r="F10" s="306"/>
+      <c r="F10" s="305"/>
       <c r="G10" s="143" t="s">
         <v>3036</v>
       </c>
       <c r="H10" s="251"/>
       <c r="I10" s="251"/>
-      <c r="K10" s="306"/>
+      <c r="K10" s="305"/>
       <c r="L10" s="143" t="s">
         <v>3029</v>
       </c>
       <c r="M10" s="251"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="358"/>
-      <c r="B11" s="306"/>
+      <c r="A11" s="360"/>
+      <c r="B11" s="305"/>
       <c r="C11" s="143"/>
       <c r="D11" s="251"/>
-      <c r="F11" s="306"/>
+      <c r="F11" s="305"/>
       <c r="G11" s="143"/>
       <c r="H11" s="251" t="s">
         <v>3032</v>
@@ -52213,24 +52275,24 @@
       <c r="J11" t="s">
         <v>3034</v>
       </c>
-      <c r="K11" s="306"/>
+      <c r="K11" s="305"/>
       <c r="L11" s="143"/>
       <c r="M11" s="251" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="358"/>
-      <c r="B12" s="306"/>
+      <c r="A12" s="360"/>
+      <c r="B12" s="305"/>
       <c r="C12" s="143"/>
       <c r="D12" s="251"/>
-      <c r="F12" s="306"/>
+      <c r="F12" s="305"/>
       <c r="G12" s="143" t="s">
         <v>137</v>
       </c>
       <c r="H12" s="251"/>
       <c r="I12" s="251"/>
-      <c r="K12" s="306"/>
+      <c r="K12" s="305"/>
       <c r="L12" s="143" t="s">
         <v>137</v>
       </c>
@@ -52240,13 +52302,13 @@
       <c r="B13" s="33"/>
       <c r="C13" s="27"/>
       <c r="D13" s="34"/>
-      <c r="F13" s="306"/>
+      <c r="F13" s="305"/>
       <c r="G13" s="143"/>
       <c r="H13" s="251" t="s">
         <v>2086</v>
       </c>
       <c r="I13" s="251"/>
-      <c r="K13" s="306"/>
+      <c r="K13" s="305"/>
       <c r="L13" s="143"/>
       <c r="M13" s="251" t="s">
         <v>2086</v>
@@ -52335,21 +52397,21 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1">
       <c r="B28" s="43"/>
-      <c r="D28" s="308"/>
-      <c r="E28" s="309"/>
-      <c r="F28" s="310"/>
+      <c r="D28" s="307"/>
+      <c r="E28" s="308"/>
+      <c r="F28" s="309"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1">
       <c r="B29" s="43"/>
-      <c r="D29" s="308"/>
-      <c r="E29" s="309"/>
-      <c r="F29" s="310"/>
+      <c r="D29" s="307"/>
+      <c r="E29" s="308"/>
+      <c r="F29" s="309"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1">
       <c r="B30" s="43"/>
-      <c r="D30" s="308"/>
-      <c r="E30" s="309"/>
-      <c r="F30" s="310"/>
+      <c r="D30" s="307"/>
+      <c r="E30" s="308"/>
+      <c r="F30" s="309"/>
     </row>
     <row r="31" spans="1:8">
       <c r="B31" s="43"/>
@@ -52400,23 +52462,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="360" t="s">
+      <c r="A1" s="362" t="s">
         <v>2598</v>
       </c>
-      <c r="B1" s="360"/>
-      <c r="C1" s="360"/>
-      <c r="D1" s="360"/>
-      <c r="E1" s="360"/>
-      <c r="F1" s="360"/>
-      <c r="I1" s="360" t="s">
+      <c r="B1" s="362"/>
+      <c r="C1" s="362"/>
+      <c r="D1" s="362"/>
+      <c r="E1" s="362"/>
+      <c r="F1" s="362"/>
+      <c r="I1" s="362" t="s">
         <v>2610</v>
       </c>
-      <c r="J1" s="360"/>
-      <c r="K1" s="360"/>
-      <c r="L1" s="360"/>
-      <c r="M1" s="360"/>
-      <c r="N1" s="360"/>
-      <c r="O1" s="360"/>
+      <c r="J1" s="362"/>
+      <c r="K1" s="362"/>
+      <c r="L1" s="362"/>
+      <c r="M1" s="362"/>
+      <c r="N1" s="362"/>
+      <c r="O1" s="362"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -52572,28 +52634,28 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A12" s="339" t="s">
+      <c r="A12" s="341" t="s">
         <v>2612</v>
       </c>
-      <c r="B12" s="359"/>
-      <c r="C12" s="359"/>
-      <c r="D12" s="359"/>
-      <c r="E12" s="359"/>
-      <c r="F12" s="359"/>
-      <c r="G12" s="359"/>
-      <c r="H12" s="340"/>
-      <c r="I12" s="339" t="s">
+      <c r="B12" s="361"/>
+      <c r="C12" s="361"/>
+      <c r="D12" s="361"/>
+      <c r="E12" s="361"/>
+      <c r="F12" s="361"/>
+      <c r="G12" s="361"/>
+      <c r="H12" s="342"/>
+      <c r="I12" s="341" t="s">
         <v>2612</v>
       </c>
-      <c r="J12" s="359"/>
-      <c r="K12" s="359"/>
-      <c r="L12" s="359"/>
-      <c r="M12" s="359"/>
-      <c r="N12" s="359"/>
-      <c r="O12" s="359"/>
-      <c r="P12" s="359"/>
-      <c r="Q12" s="359"/>
-      <c r="R12" s="340"/>
+      <c r="J12" s="361"/>
+      <c r="K12" s="361"/>
+      <c r="L12" s="361"/>
+      <c r="M12" s="361"/>
+      <c r="N12" s="361"/>
+      <c r="O12" s="361"/>
+      <c r="P12" s="361"/>
+      <c r="Q12" s="361"/>
+      <c r="R12" s="342"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="30" t="s">
@@ -52821,14 +52883,14 @@
       <c r="R21" s="37"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="360" t="s">
+      <c r="A24" s="362" t="s">
         <v>2598</v>
       </c>
-      <c r="B24" s="360"/>
-      <c r="C24" s="360"/>
-      <c r="D24" s="360"/>
-      <c r="E24" s="360"/>
-      <c r="F24" s="360"/>
+      <c r="B24" s="362"/>
+      <c r="C24" s="362"/>
+      <c r="D24" s="362"/>
+      <c r="E24" s="362"/>
+      <c r="F24" s="362"/>
       <c r="H24" s="260" t="s">
         <v>2610</v>
       </c>
@@ -52838,11 +52900,11 @@
       <c r="L24" s="260"/>
       <c r="M24" s="260"/>
       <c r="N24" s="260"/>
-      <c r="P24" s="360" t="s">
+      <c r="P24" s="362" t="s">
         <v>2651</v>
       </c>
-      <c r="Q24" s="360"/>
-      <c r="R24" s="360"/>
+      <c r="Q24" s="362"/>
+      <c r="R24" s="362"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="106" t="s">
@@ -53082,28 +53144,28 @@
       </c>
     </row>
     <row r="35" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A35" s="339" t="s">
+      <c r="A35" s="341" t="s">
         <v>2652</v>
       </c>
-      <c r="B35" s="359"/>
-      <c r="C35" s="359"/>
-      <c r="D35" s="359"/>
-      <c r="E35" s="359"/>
-      <c r="F35" s="359"/>
-      <c r="G35" s="359"/>
-      <c r="H35" s="340"/>
-      <c r="I35" s="339" t="s">
+      <c r="B35" s="361"/>
+      <c r="C35" s="361"/>
+      <c r="D35" s="361"/>
+      <c r="E35" s="361"/>
+      <c r="F35" s="361"/>
+      <c r="G35" s="361"/>
+      <c r="H35" s="342"/>
+      <c r="I35" s="341" t="s">
         <v>1113</v>
       </c>
-      <c r="J35" s="359"/>
-      <c r="K35" s="359"/>
-      <c r="L35" s="359"/>
-      <c r="M35" s="359"/>
-      <c r="N35" s="359"/>
-      <c r="O35" s="359"/>
-      <c r="P35" s="359"/>
-      <c r="Q35" s="359"/>
-      <c r="R35" s="340"/>
+      <c r="J35" s="361"/>
+      <c r="K35" s="361"/>
+      <c r="L35" s="361"/>
+      <c r="M35" s="361"/>
+      <c r="N35" s="361"/>
+      <c r="O35" s="361"/>
+      <c r="P35" s="361"/>
+      <c r="Q35" s="361"/>
+      <c r="R35" s="342"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" thickBot="1">
       <c r="A36" s="30" t="s">

</xml_diff>